<commit_message>
Korrekturen laut liste RH - Org und Place
die Korrekturen gemäß Liste erledigt, zahlreiche Fehlermeldunge konnten auf Grund von fehlenden GNDs nicht behoben werden, auch die Fehlermeldungen der json.Dateien nicht behoben bei places
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Ortsregister_2023.xlsx
+++ b/data/xlsx/Baernreither_Ortsregister_2023.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/data/xlsx/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13725"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13720"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="257">
   <si>
     <t>Reichenberg</t>
   </si>
@@ -787,6 +795,9 @@
   </si>
   <si>
     <t>key</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/12059772/budapest-vi.html</t>
   </si>
 </sst>
 </file>
@@ -882,7 +893,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1255,19 +1266,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="224" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="74.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="74.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>178</v>
       </c>
@@ -1331,7 +1342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>182</v>
       </c>
@@ -1345,7 +1356,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>132</v>
       </c>
@@ -1385,7 +1396,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>179</v>
       </c>
@@ -1411,7 +1422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
@@ -1495,7 +1506,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1509,7 +1520,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>196</v>
       </c>
@@ -1561,7 +1572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>180</v>
       </c>
@@ -1611,7 +1622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>198</v>
       </c>
@@ -1659,7 +1670,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
@@ -1673,7 +1684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>12</v>
       </c>
@@ -1685,7 +1696,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>103</v>
       </c>
@@ -1697,7 +1708,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>193</v>
       </c>
@@ -1711,7 +1722,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>194</v>
       </c>
@@ -1725,7 +1736,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
@@ -1739,7 +1750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
@@ -1753,7 +1764,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>220</v>
       </c>
@@ -1765,7 +1776,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>27</v>
       </c>
@@ -1779,7 +1790,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>54</v>
       </c>
@@ -1793,7 +1804,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>28</v>
       </c>
@@ -1805,7 +1816,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>184</v>
       </c>
@@ -1819,7 +1830,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>183</v>
       </c>
@@ -1833,7 +1844,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>55</v>
       </c>
@@ -1847,7 +1858,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>190</v>
       </c>
@@ -1861,7 +1872,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>48</v>
       </c>
@@ -1875,7 +1886,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>25</v>
       </c>
@@ -1889,7 +1900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>63</v>
       </c>
@@ -1903,7 +1914,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>42</v>
       </c>
@@ -1915,7 +1926,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>215</v>
       </c>
@@ -1929,7 +1940,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>85</v>
       </c>
@@ -1941,7 +1952,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>40</v>
       </c>
@@ -1953,7 +1964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>191</v>
       </c>
@@ -1965,7 +1976,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>44</v>
       </c>
@@ -1977,7 +1988,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>52</v>
       </c>
@@ -1991,7 +2002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>185</v>
       </c>
@@ -2005,7 +2016,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>32</v>
       </c>
@@ -2017,7 +2028,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>37</v>
       </c>
@@ -2029,7 +2040,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>57</v>
       </c>
@@ -2041,7 +2052,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>24</v>
       </c>
@@ -2055,7 +2066,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>51</v>
       </c>
@@ -2069,7 +2080,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>23</v>
       </c>
@@ -2083,7 +2094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>2</v>
       </c>
@@ -2097,7 +2108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>192</v>
       </c>
@@ -2111,7 +2122,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>211</v>
       </c>
@@ -2125,7 +2136,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>18</v>
       </c>
@@ -2151,7 +2162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>36</v>
       </c>
@@ -2163,7 +2174,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>186</v>
       </c>
@@ -2177,7 +2188,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>59</v>
       </c>
@@ -2191,7 +2202,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>5</v>
       </c>
@@ -2205,7 +2216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>188</v>
       </c>
@@ -2217,7 +2228,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>22</v>
       </c>
@@ -2229,7 +2240,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>49</v>
       </c>
@@ -2243,7 +2254,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>56</v>
       </c>
@@ -2257,7 +2268,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>6</v>
       </c>
@@ -2271,7 +2282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>206</v>
       </c>
@@ -2279,13 +2290,13 @@
         <v>97</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>207</v>
+        <v>256</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>20</v>
       </c>
@@ -2297,7 +2308,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>45</v>
       </c>
@@ -2311,7 +2322,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>17</v>
       </c>
@@ -2325,7 +2336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>19</v>
       </c>
@@ -2339,7 +2350,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>7</v>
       </c>
@@ -2353,7 +2364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>31</v>
       </c>
@@ -2367,7 +2378,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>203</v>
       </c>
@@ -2381,7 +2392,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>175</v>
       </c>
@@ -2395,7 +2406,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>1</v>
       </c>
@@ -2407,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>139</v>
       </c>
@@ -2421,7 +2432,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>101</v>
       </c>
@@ -2433,7 +2444,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>15</v>
       </c>
@@ -2484,7 +2495,7 @@
     <hyperlink ref="C64" r:id="rId33"/>
     <hyperlink ref="C87" r:id="rId34"/>
     <hyperlink ref="C85" r:id="rId35"/>
-    <hyperlink ref="C77" r:id="rId36"/>
+    <hyperlink ref="C77" r:id="rId36" display="https://www.geonames.org/3054638/budapest.html "/>
     <hyperlink ref="C75" r:id="rId37"/>
     <hyperlink ref="C65" r:id="rId38"/>
     <hyperlink ref="C61" r:id="rId39"/>

</xml_diff>

<commit_message>
Correction according to list and for Lesefassung
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Ortsregister_2023.xlsx
+++ b/data/xlsx/Baernreither_Ortsregister_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB55F30-D1A4-8449-85B4-4F9A51D39F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B985574-6997-BA41-81D0-10C45236BCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="850">
   <si>
     <t>Name</t>
   </si>
@@ -1340,9 +1340,6 @@
     <t>München</t>
   </si>
   <si>
-    <t>http://www.geonames.org/2867714/munich.html</t>
-  </si>
-  <si>
     <t>Muenchen</t>
   </si>
   <si>
@@ -1547,9 +1544,6 @@
     <t>Olomouc</t>
   </si>
   <si>
-    <t>http://www.geonames.org/3069011/olomouc.html</t>
-  </si>
-  <si>
     <t>Olmuetz</t>
   </si>
   <si>
@@ -1700,9 +1694,6 @@
     <t>https://www.geonames.org/8987776/predel.html</t>
   </si>
   <si>
-    <t>Preußen</t>
-  </si>
-  <si>
     <t>Propyläen</t>
   </si>
   <si>
@@ -1953,12 +1944,6 @@
   </si>
   <si>
     <t>SchleswigHolstein</t>
-  </si>
-  <si>
-    <t>Schütt</t>
-  </si>
-  <si>
-    <t>Schuett</t>
   </si>
   <si>
     <t xml:space="preserve">Schwarzwasser </t>
@@ -2587,6 +2572,12 @@
   </si>
   <si>
     <t>https://www.geonames.org/12059772/budapest-vi.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/6559171/muenchen-landeshauptstadt.html</t>
+  </si>
+  <si>
+    <t>https://www.geonames.org/3069011/olomouc.html</t>
   </si>
 </sst>
 </file>
@@ -2885,7 +2876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3047,6 +3038,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -3097,7 +3091,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E314" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E312" headerRowCount="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -3312,10 +3306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1224"/>
+  <dimension ref="A1:Z1222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="169" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="169" workbookViewId="0">
+      <selection activeCell="A241" sqref="A241:XFD241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -7810,7 +7804,7 @@
       </c>
       <c r="B130" s="30"/>
       <c r="C130" s="57" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>338</v>
@@ -8330,14 +8324,14 @@
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1">
       <c r="A145" s="6" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="B145" s="6"/>
       <c r="C145" s="6" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="E145" s="6"/>
       <c r="F145" s="2"/>
@@ -9100,10 +9094,10 @@
       </c>
       <c r="B167" s="6"/>
       <c r="C167" s="15" t="s">
+        <v>848</v>
+      </c>
+      <c r="D167" s="6" t="s">
         <v>437</v>
-      </c>
-      <c r="D167" s="6" t="s">
-        <v>438</v>
       </c>
       <c r="E167" s="6"/>
       <c r="F167" s="2"/>
@@ -9130,16 +9124,16 @@
     </row>
     <row r="168" spans="1:26" ht="15.75" customHeight="1">
       <c r="A168" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="B168" s="20" t="s">
         <v>439</v>
       </c>
-      <c r="B168" s="20" t="s">
+      <c r="C168" s="13" t="s">
         <v>440</v>
       </c>
-      <c r="C168" s="13" t="s">
-        <v>441</v>
-      </c>
       <c r="D168" s="12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E168" s="12"/>
       <c r="F168" s="5"/>
@@ -9166,14 +9160,14 @@
     </row>
     <row r="169" spans="1:26" ht="15.75" customHeight="1">
       <c r="A169" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B169" s="12"/>
       <c r="C169" s="13" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D169" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E169" s="12"/>
       <c r="F169" s="5"/>
@@ -9200,16 +9194,16 @@
     </row>
     <row r="170" spans="1:26" ht="15.75" customHeight="1">
       <c r="A170" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="B170" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="B170" s="12" t="s">
+      <c r="C170" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="C170" s="14" t="s">
-        <v>446</v>
-      </c>
       <c r="D170" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E170" s="12"/>
       <c r="F170" s="5"/>
@@ -9236,16 +9230,16 @@
     </row>
     <row r="171" spans="1:26" ht="15.75" customHeight="1">
       <c r="A171" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="B171" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="B171" s="12" t="s">
+      <c r="C171" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="C171" s="13" t="s">
-        <v>449</v>
-      </c>
       <c r="D171" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E171" s="12"/>
       <c r="F171" s="5"/>
@@ -9272,16 +9266,16 @@
     </row>
     <row r="172" spans="1:26" ht="15.75" customHeight="1">
       <c r="A172" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="B172" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B172" s="6" t="s">
+      <c r="C172" s="56" t="s">
+        <v>843</v>
+      </c>
+      <c r="D172" s="6" t="s">
         <v>451</v>
-      </c>
-      <c r="C172" s="56" t="s">
-        <v>848</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>452</v>
       </c>
       <c r="E172" s="6"/>
       <c r="F172" s="2"/>
@@ -9308,14 +9302,14 @@
     </row>
     <row r="173" spans="1:26" ht="15.75" customHeight="1">
       <c r="A173" s="12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B173" s="12"/>
       <c r="C173" s="36" t="s">
+        <v>453</v>
+      </c>
+      <c r="D173" s="37" t="s">
         <v>454</v>
-      </c>
-      <c r="D173" s="37" t="s">
-        <v>455</v>
       </c>
       <c r="E173" s="37"/>
       <c r="F173" s="5"/>
@@ -9342,14 +9336,14 @@
     </row>
     <row r="174" spans="1:26" ht="15.75" customHeight="1">
       <c r="A174" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B174" s="6"/>
       <c r="C174" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="D174" s="6" t="s">
         <v>457</v>
-      </c>
-      <c r="D174" s="6" t="s">
-        <v>458</v>
       </c>
       <c r="E174" s="6"/>
       <c r="F174" s="2"/>
@@ -9376,14 +9370,14 @@
     </row>
     <row r="175" spans="1:26" ht="15.75" customHeight="1">
       <c r="A175" s="12" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B175" s="12"/>
       <c r="C175" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="D175" s="12" t="s">
         <v>460</v>
-      </c>
-      <c r="D175" s="12" t="s">
-        <v>461</v>
       </c>
       <c r="E175" s="12"/>
       <c r="F175" s="5"/>
@@ -9410,16 +9404,16 @@
     </row>
     <row r="176" spans="1:26" ht="15.75" customHeight="1">
       <c r="A176" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="B176" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="B176" s="10" t="s">
+      <c r="C176" s="32" t="s">
         <v>463</v>
       </c>
-      <c r="C176" s="32" t="s">
-        <v>464</v>
-      </c>
       <c r="D176" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E176" s="10"/>
       <c r="F176" s="2"/>
@@ -9446,16 +9440,16 @@
     </row>
     <row r="177" spans="1:26" ht="15.75" customHeight="1">
       <c r="A177" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="B177" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="B177" s="8" t="s">
+      <c r="C177" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="C177" s="9" t="s">
-        <v>467</v>
-      </c>
       <c r="D177" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E177" s="10"/>
       <c r="F177" s="2"/>
@@ -9482,16 +9476,16 @@
     </row>
     <row r="178" spans="1:26" ht="15.75" customHeight="1">
       <c r="A178" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="B178" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="C178" s="32" t="s">
         <v>468</v>
       </c>
-      <c r="B178" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="C178" s="32" t="s">
-        <v>469</v>
-      </c>
       <c r="D178" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E178" s="10"/>
       <c r="F178" s="2"/>
@@ -9518,14 +9512,14 @@
     </row>
     <row r="179" spans="1:26" ht="15.75" customHeight="1">
       <c r="A179" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B179" s="6"/>
       <c r="C179" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D179" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E179" s="6"/>
       <c r="F179" s="2"/>
@@ -9552,14 +9546,14 @@
     </row>
     <row r="180" spans="1:26" ht="15.75" customHeight="1">
       <c r="A180" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B180" s="10"/>
       <c r="C180" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E180" s="6"/>
       <c r="F180" s="2"/>
@@ -9586,14 +9580,14 @@
     </row>
     <row r="181" spans="1:26" ht="15.75" customHeight="1">
       <c r="A181" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B181" s="6"/>
       <c r="C181" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="D181" s="6" t="s">
         <v>475</v>
-      </c>
-      <c r="D181" s="6" t="s">
-        <v>476</v>
       </c>
       <c r="E181" s="6"/>
       <c r="F181" s="2"/>
@@ -9620,14 +9614,14 @@
     </row>
     <row r="182" spans="1:26" ht="15.75" customHeight="1">
       <c r="A182" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B182" s="10"/>
       <c r="C182" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="D182" s="10" t="s">
         <v>478</v>
-      </c>
-      <c r="D182" s="10" t="s">
-        <v>479</v>
       </c>
       <c r="E182" s="6"/>
       <c r="F182" s="2"/>
@@ -9654,14 +9648,14 @@
     </row>
     <row r="183" spans="1:26" ht="15.75" customHeight="1">
       <c r="A183" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B183" s="6"/>
       <c r="C183" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E183" s="6"/>
       <c r="F183" s="2"/>
@@ -9688,14 +9682,14 @@
     </row>
     <row r="184" spans="1:26" ht="15.75" customHeight="1">
       <c r="A184" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B184" s="10"/>
       <c r="C184" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="D184" s="10" t="s">
         <v>483</v>
-      </c>
-      <c r="D184" s="10" t="s">
-        <v>484</v>
       </c>
       <c r="E184" s="10"/>
       <c r="F184" s="2"/>
@@ -9722,16 +9716,16 @@
     </row>
     <row r="185" spans="1:26" ht="15.75" customHeight="1">
       <c r="A185" s="38" t="s">
+        <v>484</v>
+      </c>
+      <c r="B185" s="38" t="s">
         <v>485</v>
       </c>
-      <c r="B185" s="38" t="s">
+      <c r="C185" s="39" t="s">
         <v>486</v>
       </c>
-      <c r="C185" s="39" t="s">
-        <v>487</v>
-      </c>
       <c r="D185" s="38" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E185" s="40"/>
       <c r="F185" s="2"/>
@@ -9758,16 +9752,16 @@
     </row>
     <row r="186" spans="1:26" ht="15.75" customHeight="1">
       <c r="A186" s="38" t="s">
+        <v>487</v>
+      </c>
+      <c r="B186" s="38" t="s">
         <v>488</v>
       </c>
-      <c r="B186" s="38" t="s">
+      <c r="C186" s="41" t="s">
         <v>489</v>
       </c>
-      <c r="C186" s="41" t="s">
+      <c r="D186" s="38" t="s">
         <v>490</v>
-      </c>
-      <c r="D186" s="38" t="s">
-        <v>491</v>
       </c>
       <c r="E186" s="40"/>
       <c r="F186" s="2"/>
@@ -9794,16 +9788,16 @@
     </row>
     <row r="187" spans="1:26" ht="15.75" customHeight="1">
       <c r="A187" s="38" t="s">
+        <v>491</v>
+      </c>
+      <c r="B187" s="38" t="s">
         <v>492</v>
       </c>
-      <c r="B187" s="38" t="s">
+      <c r="C187" s="41" t="s">
         <v>493</v>
       </c>
-      <c r="C187" s="41" t="s">
-        <v>494</v>
-      </c>
       <c r="D187" s="38" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E187" s="40"/>
       <c r="F187" s="2"/>
@@ -9830,16 +9824,16 @@
     </row>
     <row r="188" spans="1:26" ht="15.75" customHeight="1">
       <c r="A188" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="B188" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="B188" s="6" t="s">
+      <c r="C188" s="15" t="s">
         <v>496</v>
       </c>
-      <c r="C188" s="15" t="s">
-        <v>497</v>
-      </c>
       <c r="D188" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E188" s="6"/>
       <c r="F188" s="2"/>
@@ -9866,14 +9860,14 @@
     </row>
     <row r="189" spans="1:26" ht="15.75" customHeight="1">
       <c r="A189" s="10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B189" s="10"/>
       <c r="C189" s="11" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E189" s="6"/>
       <c r="F189" s="2"/>
@@ -9900,16 +9894,16 @@
     </row>
     <row r="190" spans="1:26" ht="15.75" customHeight="1">
       <c r="A190" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="B190" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="B190" s="8" t="s">
+      <c r="C190" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="C190" s="9" t="s">
+      <c r="D190" s="8" t="s">
         <v>502</v>
-      </c>
-      <c r="D190" s="8" t="s">
-        <v>503</v>
       </c>
       <c r="E190" s="6"/>
       <c r="F190" s="2"/>
@@ -9936,16 +9930,16 @@
     </row>
     <row r="191" spans="1:26" ht="15.75" customHeight="1">
       <c r="A191" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="B191" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="B191" s="6" t="s">
+      <c r="C191" s="56" t="s">
+        <v>849</v>
+      </c>
+      <c r="D191" s="6" t="s">
         <v>505</v>
-      </c>
-      <c r="C191" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="D191" s="6" t="s">
-        <v>507</v>
       </c>
       <c r="E191" s="6"/>
       <c r="F191" s="2"/>
@@ -9972,14 +9966,14 @@
     </row>
     <row r="192" spans="1:26" ht="15.75" customHeight="1">
       <c r="A192" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B192" s="8"/>
       <c r="C192" s="33" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E192" s="6"/>
       <c r="F192" s="2"/>
@@ -10006,14 +10000,14 @@
     </row>
     <row r="193" spans="1:26" ht="15.75" customHeight="1">
       <c r="A193" s="6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B193" s="6"/>
       <c r="C193" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E193" s="6"/>
       <c r="F193" s="2"/>
@@ -10040,14 +10034,14 @@
     </row>
     <row r="194" spans="1:26" ht="15.75" customHeight="1">
       <c r="A194" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B194" s="6"/>
       <c r="C194" s="7" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E194" s="6"/>
       <c r="F194" s="2"/>
@@ -10074,14 +10068,14 @@
     </row>
     <row r="195" spans="1:26" ht="15.75" customHeight="1">
       <c r="A195" s="12" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B195" s="42"/>
       <c r="C195" s="14" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D195" s="37" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E195" s="43"/>
       <c r="F195" s="44"/>
@@ -10108,14 +10102,14 @@
     </row>
     <row r="196" spans="1:26" ht="15.75" customHeight="1">
       <c r="A196" s="8" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B196" s="8"/>
       <c r="C196" s="9" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E196" s="6"/>
       <c r="F196" s="2"/>
@@ -10142,14 +10136,14 @@
     </row>
     <row r="197" spans="1:26" ht="15.75" customHeight="1">
       <c r="A197" s="6" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B197" s="6"/>
       <c r="C197" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E197" s="6"/>
       <c r="F197" s="2"/>
@@ -10176,14 +10170,14 @@
     </row>
     <row r="198" spans="1:26" ht="15.75" customHeight="1">
       <c r="A198" s="10" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B198" s="10"/>
       <c r="C198" s="32" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E198" s="10"/>
       <c r="F198" s="2"/>
@@ -10210,16 +10204,16 @@
     </row>
     <row r="199" spans="1:26" ht="15.75" customHeight="1">
       <c r="A199" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="C199" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="B199" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="C199" s="6" t="s">
-        <v>525</v>
-      </c>
       <c r="D199" s="6" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E199" s="6"/>
       <c r="F199" s="2"/>
@@ -10246,14 +10240,14 @@
     </row>
     <row r="200" spans="1:26" ht="15.75" customHeight="1">
       <c r="A200" s="10" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B200" s="10"/>
       <c r="C200" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D200" s="10" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E200" s="10"/>
       <c r="F200" s="2"/>
@@ -10280,16 +10274,16 @@
     </row>
     <row r="201" spans="1:26" ht="15.75" customHeight="1">
       <c r="A201" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="C201" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="B201" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="C201" s="9" t="s">
-        <v>530</v>
-      </c>
       <c r="D201" s="8" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E201" s="6"/>
       <c r="F201" s="2"/>
@@ -10316,16 +10310,16 @@
     </row>
     <row r="202" spans="1:26" ht="15.75" customHeight="1">
       <c r="A202" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="C202" s="15" t="s">
         <v>531</v>
       </c>
-      <c r="B202" s="6" t="s">
-        <v>532</v>
-      </c>
-      <c r="C202" s="15" t="s">
-        <v>533</v>
-      </c>
       <c r="D202" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E202" s="6"/>
       <c r="F202" s="2"/>
@@ -10352,16 +10346,16 @@
     </row>
     <row r="203" spans="1:26" ht="15.75" customHeight="1">
       <c r="A203" s="12" t="s">
+        <v>532</v>
+      </c>
+      <c r="B203" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="C203" s="59" t="s">
         <v>534</v>
       </c>
-      <c r="B203" s="12" t="s">
-        <v>535</v>
-      </c>
-      <c r="C203" s="13" t="s">
-        <v>536</v>
-      </c>
       <c r="D203" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E203" s="12"/>
       <c r="F203" s="5"/>
@@ -10388,14 +10382,14 @@
     </row>
     <row r="204" spans="1:26" ht="15.75" customHeight="1">
       <c r="A204" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B204" s="12"/>
       <c r="C204" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D204" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E204" s="12"/>
       <c r="F204" s="5"/>
@@ -10422,16 +10416,16 @@
     </row>
     <row r="205" spans="1:26" ht="15.75" customHeight="1">
       <c r="A205" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="C205" s="6" t="s">
         <v>539</v>
       </c>
-      <c r="B205" s="6" t="s">
-        <v>540</v>
-      </c>
-      <c r="C205" s="6" t="s">
-        <v>541</v>
-      </c>
       <c r="D205" s="6" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E205" s="6"/>
       <c r="F205" s="2"/>
@@ -10458,14 +10452,14 @@
     </row>
     <row r="206" spans="1:26" ht="15.75" customHeight="1">
       <c r="A206" s="8" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B206" s="8"/>
       <c r="C206" s="9" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E206" s="10"/>
       <c r="F206" s="2"/>
@@ -10492,16 +10486,16 @@
     </row>
     <row r="207" spans="1:26" ht="15.75" customHeight="1">
       <c r="A207" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="B207" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="C207" s="11" t="s">
         <v>544</v>
       </c>
-      <c r="B207" s="10" t="s">
-        <v>545</v>
-      </c>
-      <c r="C207" s="11" t="s">
-        <v>546</v>
-      </c>
       <c r="D207" s="10" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E207" s="10"/>
       <c r="F207" s="2"/>
@@ -10528,16 +10522,16 @@
     </row>
     <row r="208" spans="1:26" ht="15.75" customHeight="1">
       <c r="A208" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="B208" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="C208" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="B208" s="12" t="s">
+      <c r="D208" s="12" t="s">
         <v>548</v>
-      </c>
-      <c r="C208" s="13" t="s">
-        <v>549</v>
-      </c>
-      <c r="D208" s="12" t="s">
-        <v>550</v>
       </c>
       <c r="E208" s="12"/>
       <c r="F208" s="5"/>
@@ -10564,16 +10558,16 @@
     </row>
     <row r="209" spans="1:26" ht="15.75" customHeight="1">
       <c r="A209" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="C209" s="15" t="s">
         <v>551</v>
       </c>
-      <c r="B209" s="6" t="s">
-        <v>552</v>
-      </c>
-      <c r="C209" s="15" t="s">
-        <v>553</v>
-      </c>
       <c r="D209" s="6" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E209" s="6"/>
       <c r="F209" s="2"/>
@@ -10600,16 +10594,16 @@
     </row>
     <row r="210" spans="1:26" ht="15.75" customHeight="1">
       <c r="A210" s="12" t="s">
+        <v>552</v>
+      </c>
+      <c r="B210" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="C210" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="B210" s="12" t="s">
-        <v>555</v>
-      </c>
-      <c r="C210" s="36" t="s">
-        <v>556</v>
-      </c>
       <c r="D210" s="37" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E210" s="37"/>
       <c r="F210" s="5"/>
@@ -10635,12 +10629,14 @@
       <c r="Z210" s="5"/>
     </row>
     <row r="211" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A211" s="12" t="s">
-        <v>557</v>
-      </c>
-      <c r="B211" s="12"/>
-      <c r="C211" s="36"/>
-      <c r="D211" s="37" t="s">
+      <c r="A211" s="16" t="s">
+        <v>555</v>
+      </c>
+      <c r="B211" s="16"/>
+      <c r="C211" s="45" t="s">
+        <v>556</v>
+      </c>
+      <c r="D211" s="46" t="s">
         <v>557</v>
       </c>
       <c r="E211" s="37"/>
@@ -10667,15 +10663,17 @@
       <c r="Z211" s="5"/>
     </row>
     <row r="212" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A212" s="16" t="s">
+      <c r="A212" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="B212" s="16"/>
-      <c r="C212" s="45" t="s">
+      <c r="B212" s="12" t="s">
         <v>559</v>
       </c>
-      <c r="D212" s="46" t="s">
+      <c r="C212" s="47" t="s">
         <v>560</v>
+      </c>
+      <c r="D212" s="37" t="s">
+        <v>558</v>
       </c>
       <c r="E212" s="37"/>
       <c r="F212" s="5"/>
@@ -10701,87 +10699,87 @@
       <c r="Z212" s="5"/>
     </row>
     <row r="213" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A213" s="12" t="s">
+      <c r="A213" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="B213" s="12" t="s">
+      <c r="B213" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="C213" s="47" t="s">
+      <c r="C213" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="D213" s="37" t="s">
-        <v>561</v>
-      </c>
-      <c r="E213" s="37"/>
-      <c r="F213" s="5"/>
-      <c r="G213" s="5"/>
-      <c r="H213" s="5"/>
-      <c r="I213" s="5"/>
-      <c r="J213" s="5"/>
-      <c r="K213" s="5"/>
-      <c r="L213" s="5"/>
-      <c r="M213" s="5"/>
-      <c r="N213" s="5"/>
-      <c r="O213" s="5"/>
-      <c r="P213" s="5"/>
-      <c r="Q213" s="5"/>
-      <c r="R213" s="5"/>
-      <c r="S213" s="5"/>
-      <c r="T213" s="5"/>
-      <c r="U213" s="5"/>
-      <c r="V213" s="5"/>
-      <c r="W213" s="5"/>
-      <c r="X213" s="5"/>
-      <c r="Y213" s="5"/>
-      <c r="Z213" s="5"/>
+      <c r="D213" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="E213" s="6"/>
+      <c r="F213" s="2"/>
+      <c r="G213" s="2"/>
+      <c r="H213" s="2"/>
+      <c r="I213" s="2"/>
+      <c r="J213" s="2"/>
+      <c r="K213" s="2"/>
+      <c r="L213" s="2"/>
+      <c r="M213" s="2"/>
+      <c r="N213" s="2"/>
+      <c r="O213" s="2"/>
+      <c r="P213" s="2"/>
+      <c r="Q213" s="2"/>
+      <c r="R213" s="2"/>
+      <c r="S213" s="2"/>
+      <c r="T213" s="2"/>
+      <c r="U213" s="2"/>
+      <c r="V213" s="2"/>
+      <c r="W213" s="2"/>
+      <c r="X213" s="2"/>
+      <c r="Y213" s="2"/>
+      <c r="Z213" s="2"/>
     </row>
     <row r="214" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A214" s="6" t="s">
+      <c r="A214" s="12" t="s">
         <v>564</v>
       </c>
-      <c r="B214" s="6" t="s">
+      <c r="B214" s="12"/>
+      <c r="C214" s="37" t="s">
         <v>565</v>
       </c>
-      <c r="C214" s="7" t="s">
+      <c r="D214" s="12" t="s">
         <v>566</v>
       </c>
-      <c r="D214" s="6" t="s">
-        <v>565</v>
-      </c>
-      <c r="E214" s="6"/>
-      <c r="F214" s="2"/>
-      <c r="G214" s="2"/>
-      <c r="H214" s="2"/>
-      <c r="I214" s="2"/>
-      <c r="J214" s="2"/>
-      <c r="K214" s="2"/>
-      <c r="L214" s="2"/>
-      <c r="M214" s="2"/>
-      <c r="N214" s="2"/>
-      <c r="O214" s="2"/>
-      <c r="P214" s="2"/>
-      <c r="Q214" s="2"/>
-      <c r="R214" s="2"/>
-      <c r="S214" s="2"/>
-      <c r="T214" s="2"/>
-      <c r="U214" s="2"/>
-      <c r="V214" s="2"/>
-      <c r="W214" s="2"/>
-      <c r="X214" s="2"/>
-      <c r="Y214" s="2"/>
-      <c r="Z214" s="2"/>
+      <c r="E214" s="12"/>
+      <c r="F214" s="5"/>
+      <c r="G214" s="5"/>
+      <c r="H214" s="5"/>
+      <c r="I214" s="5"/>
+      <c r="J214" s="5"/>
+      <c r="K214" s="5"/>
+      <c r="L214" s="5"/>
+      <c r="M214" s="5"/>
+      <c r="N214" s="5"/>
+      <c r="O214" s="5"/>
+      <c r="P214" s="5"/>
+      <c r="Q214" s="5"/>
+      <c r="R214" s="5"/>
+      <c r="S214" s="5"/>
+      <c r="T214" s="5"/>
+      <c r="U214" s="5"/>
+      <c r="V214" s="5"/>
+      <c r="W214" s="5"/>
+      <c r="X214" s="5"/>
+      <c r="Y214" s="5"/>
+      <c r="Z214" s="5"/>
     </row>
     <row r="215" spans="1:26" ht="15.75" customHeight="1">
       <c r="A215" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="B215" s="12"/>
+      <c r="B215" s="12" t="s">
+        <v>568</v>
+      </c>
       <c r="C215" s="37" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D215" s="12" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E215" s="12"/>
       <c r="F215" s="5"/>
@@ -10807,124 +10805,122 @@
       <c r="Z215" s="5"/>
     </row>
     <row r="216" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A216" s="12" t="s">
-        <v>570</v>
-      </c>
-      <c r="B216" s="12" t="s">
+      <c r="A216" s="48" t="s">
         <v>571</v>
       </c>
-      <c r="C216" s="37" t="s">
+      <c r="B216" s="48" t="s">
+        <v>334</v>
+      </c>
+      <c r="C216" s="49" t="s">
+        <v>335</v>
+      </c>
+      <c r="D216" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="E216" s="50"/>
+      <c r="F216" s="2"/>
+      <c r="G216" s="2"/>
+      <c r="H216" s="2"/>
+      <c r="I216" s="2"/>
+      <c r="J216" s="2"/>
+      <c r="K216" s="2"/>
+      <c r="L216" s="2"/>
+      <c r="M216" s="2"/>
+      <c r="N216" s="2"/>
+      <c r="O216" s="2"/>
+      <c r="P216" s="2"/>
+      <c r="Q216" s="2"/>
+      <c r="R216" s="2"/>
+      <c r="S216" s="2"/>
+      <c r="T216" s="2"/>
+      <c r="U216" s="2"/>
+      <c r="V216" s="2"/>
+      <c r="W216" s="2"/>
+      <c r="X216" s="2"/>
+      <c r="Y216" s="2"/>
+      <c r="Z216" s="2"/>
+    </row>
+    <row r="217" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A217" s="12" t="s">
         <v>572</v>
       </c>
-      <c r="D216" s="12" t="s">
+      <c r="B217" s="12" t="s">
         <v>573</v>
       </c>
-      <c r="E216" s="12"/>
-      <c r="F216" s="5"/>
-      <c r="G216" s="5"/>
-      <c r="H216" s="5"/>
-      <c r="I216" s="5"/>
-      <c r="J216" s="5"/>
-      <c r="K216" s="5"/>
-      <c r="L216" s="5"/>
-      <c r="M216" s="5"/>
-      <c r="N216" s="5"/>
-      <c r="O216" s="5"/>
-      <c r="P216" s="5"/>
-      <c r="Q216" s="5"/>
-      <c r="R216" s="5"/>
-      <c r="S216" s="5"/>
-      <c r="T216" s="5"/>
-      <c r="U216" s="5"/>
-      <c r="V216" s="5"/>
-      <c r="W216" s="5"/>
-      <c r="X216" s="5"/>
-      <c r="Y216" s="5"/>
-      <c r="Z216" s="5"/>
-    </row>
-    <row r="217" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A217" s="48" t="s">
+      <c r="C217" s="37" t="s">
         <v>574</v>
       </c>
-      <c r="B217" s="48" t="s">
-        <v>334</v>
-      </c>
-      <c r="C217" s="49" t="s">
-        <v>335</v>
-      </c>
-      <c r="D217" s="48" t="s">
-        <v>574</v>
-      </c>
-      <c r="E217" s="50"/>
-      <c r="F217" s="2"/>
-      <c r="G217" s="2"/>
-      <c r="H217" s="2"/>
-      <c r="I217" s="2"/>
-      <c r="J217" s="2"/>
-      <c r="K217" s="2"/>
-      <c r="L217" s="2"/>
-      <c r="M217" s="2"/>
-      <c r="N217" s="2"/>
-      <c r="O217" s="2"/>
-      <c r="P217" s="2"/>
-      <c r="Q217" s="2"/>
-      <c r="R217" s="2"/>
-      <c r="S217" s="2"/>
-      <c r="T217" s="2"/>
-      <c r="U217" s="2"/>
-      <c r="V217" s="2"/>
-      <c r="W217" s="2"/>
-      <c r="X217" s="2"/>
-      <c r="Y217" s="2"/>
-      <c r="Z217" s="2"/>
+      <c r="D217" s="12" t="s">
+        <v>572</v>
+      </c>
+      <c r="E217" s="12"/>
+      <c r="F217" s="5"/>
+      <c r="G217" s="5"/>
+      <c r="H217" s="5"/>
+      <c r="I217" s="5"/>
+      <c r="J217" s="5"/>
+      <c r="K217" s="5"/>
+      <c r="L217" s="5"/>
+      <c r="M217" s="5"/>
+      <c r="N217" s="5"/>
+      <c r="O217" s="5"/>
+      <c r="P217" s="5"/>
+      <c r="Q217" s="5"/>
+      <c r="R217" s="5"/>
+      <c r="S217" s="5"/>
+      <c r="T217" s="5"/>
+      <c r="U217" s="5"/>
+      <c r="V217" s="5"/>
+      <c r="W217" s="5"/>
+      <c r="X217" s="5"/>
+      <c r="Y217" s="5"/>
+      <c r="Z217" s="5"/>
     </row>
     <row r="218" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A218" s="12" t="s">
+      <c r="A218" s="6" t="s">
         <v>575</v>
       </c>
-      <c r="B218" s="12" t="s">
+      <c r="B218" s="6" t="s">
+        <v>844</v>
+      </c>
+      <c r="C218" s="7" t="s">
+        <v>845</v>
+      </c>
+      <c r="D218" s="6" t="s">
         <v>576</v>
       </c>
-      <c r="C218" s="37" t="s">
+      <c r="E218" s="6"/>
+      <c r="F218" s="2"/>
+      <c r="G218" s="2"/>
+      <c r="H218" s="2"/>
+      <c r="I218" s="2"/>
+      <c r="J218" s="2"/>
+      <c r="K218" s="2"/>
+      <c r="L218" s="2"/>
+      <c r="M218" s="2"/>
+      <c r="N218" s="2"/>
+      <c r="O218" s="2"/>
+      <c r="P218" s="2"/>
+      <c r="Q218" s="2"/>
+      <c r="R218" s="2"/>
+      <c r="S218" s="2"/>
+      <c r="T218" s="2"/>
+      <c r="U218" s="2"/>
+      <c r="V218" s="2"/>
+      <c r="W218" s="2"/>
+      <c r="X218" s="2"/>
+      <c r="Y218" s="2"/>
+      <c r="Z218" s="2"/>
+    </row>
+    <row r="219" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A219" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="D218" s="12" t="s">
-        <v>575</v>
-      </c>
-      <c r="E218" s="12"/>
-      <c r="F218" s="5"/>
-      <c r="G218" s="5"/>
-      <c r="H218" s="5"/>
-      <c r="I218" s="5"/>
-      <c r="J218" s="5"/>
-      <c r="K218" s="5"/>
-      <c r="L218" s="5"/>
-      <c r="M218" s="5"/>
-      <c r="N218" s="5"/>
-      <c r="O218" s="5"/>
-      <c r="P218" s="5"/>
-      <c r="Q218" s="5"/>
-      <c r="R218" s="5"/>
-      <c r="S218" s="5"/>
-      <c r="T218" s="5"/>
-      <c r="U218" s="5"/>
-      <c r="V218" s="5"/>
-      <c r="W218" s="5"/>
-      <c r="X218" s="5"/>
-      <c r="Y218" s="5"/>
-      <c r="Z218" s="5"/>
-    </row>
-    <row r="219" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A219" s="6" t="s">
+      <c r="B219" s="10"/>
+      <c r="C219" s="11" t="s">
         <v>578</v>
       </c>
-      <c r="B219" s="6" t="s">
-        <v>849</v>
-      </c>
-      <c r="C219" s="7" t="s">
-        <v>850</v>
-      </c>
-      <c r="D219" s="6" t="s">
+      <c r="D219" s="10" t="s">
         <v>579</v>
       </c>
       <c r="E219" s="6"/>
@@ -10951,15 +10947,17 @@
       <c r="Z219" s="2"/>
     </row>
     <row r="220" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A220" s="10" t="s">
+      <c r="A220" s="8" t="s">
         <v>580</v>
       </c>
-      <c r="B220" s="10"/>
-      <c r="C220" s="11" t="s">
+      <c r="B220" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="D220" s="10" t="s">
+      <c r="C220" s="9" t="s">
         <v>582</v>
+      </c>
+      <c r="D220" s="8" t="s">
+        <v>580</v>
       </c>
       <c r="E220" s="6"/>
       <c r="F220" s="2"/>
@@ -10985,16 +10983,16 @@
       <c r="Z220" s="2"/>
     </row>
     <row r="221" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A221" s="8" t="s">
+      <c r="A221" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="B221" s="8" t="s">
+      <c r="B221" s="6" t="s">
         <v>584</v>
       </c>
-      <c r="C221" s="9" t="s">
+      <c r="C221" s="6" t="s">
         <v>585</v>
       </c>
-      <c r="D221" s="8" t="s">
+      <c r="D221" s="6" t="s">
         <v>583</v>
       </c>
       <c r="E221" s="6"/>
@@ -11021,19 +11019,17 @@
       <c r="Z221" s="2"/>
     </row>
     <row r="222" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A222" s="6" t="s">
+      <c r="A222" s="10" t="s">
         <v>586</v>
       </c>
-      <c r="B222" s="6" t="s">
+      <c r="B222" s="10"/>
+      <c r="C222" s="32" t="s">
         <v>587</v>
       </c>
-      <c r="C222" s="6" t="s">
-        <v>588</v>
-      </c>
-      <c r="D222" s="6" t="s">
+      <c r="D222" s="10" t="s">
         <v>586</v>
       </c>
-      <c r="E222" s="6"/>
+      <c r="E222" s="10"/>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
       <c r="H222" s="2"/>
@@ -11057,15 +11053,17 @@
       <c r="Z222" s="2"/>
     </row>
     <row r="223" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A223" s="10" t="s">
+      <c r="A223" s="8" t="s">
+        <v>588</v>
+      </c>
+      <c r="B223" s="8" t="s">
         <v>589</v>
       </c>
-      <c r="B223" s="10"/>
-      <c r="C223" s="32" t="s">
+      <c r="C223" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="D223" s="10" t="s">
-        <v>589</v>
+      <c r="D223" s="8" t="s">
+        <v>588</v>
       </c>
       <c r="E223" s="10"/>
       <c r="F223" s="2"/>
@@ -11091,17 +11089,17 @@
       <c r="Z223" s="2"/>
     </row>
     <row r="224" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A224" s="8" t="s">
+      <c r="A224" s="10" t="s">
         <v>591</v>
       </c>
-      <c r="B224" s="8" t="s">
+      <c r="B224" s="10" t="s">
         <v>592</v>
       </c>
-      <c r="C224" s="9" t="s">
+      <c r="C224" s="32" t="s">
         <v>593</v>
       </c>
-      <c r="D224" s="8" t="s">
-        <v>591</v>
+      <c r="D224" s="10" t="s">
+        <v>594</v>
       </c>
       <c r="E224" s="10"/>
       <c r="F224" s="2"/>
@@ -11127,19 +11125,17 @@
       <c r="Z224" s="2"/>
     </row>
     <row r="225" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A225" s="10" t="s">
-        <v>594</v>
-      </c>
-      <c r="B225" s="10" t="s">
+      <c r="A225" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="C225" s="32" t="s">
+      <c r="B225" s="8"/>
+      <c r="C225" s="9" t="s">
         <v>596</v>
       </c>
-      <c r="D225" s="10" t="s">
-        <v>597</v>
-      </c>
-      <c r="E225" s="10"/>
+      <c r="D225" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="E225" s="6"/>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
       <c r="H225" s="2"/>
@@ -11163,15 +11159,15 @@
       <c r="Z225" s="2"/>
     </row>
     <row r="226" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A226" s="8" t="s">
+      <c r="A226" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="B226" s="6"/>
+      <c r="C226" s="6" t="s">
         <v>598</v>
       </c>
-      <c r="B226" s="8"/>
-      <c r="C226" s="9" t="s">
-        <v>599</v>
-      </c>
-      <c r="D226" s="8" t="s">
-        <v>598</v>
+      <c r="D226" s="6" t="s">
+        <v>597</v>
       </c>
       <c r="E226" s="6"/>
       <c r="F226" s="2"/>
@@ -11197,15 +11193,17 @@
       <c r="Z226" s="2"/>
     </row>
     <row r="227" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A227" s="6" t="s">
+      <c r="A227" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="B227" s="8" t="s">
         <v>600</v>
       </c>
-      <c r="B227" s="6"/>
-      <c r="C227" s="6" t="s">
+      <c r="C227" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="D227" s="6" t="s">
-        <v>600</v>
+      <c r="D227" s="8" t="s">
+        <v>602</v>
       </c>
       <c r="E227" s="6"/>
       <c r="F227" s="2"/>
@@ -11231,17 +11229,15 @@
       <c r="Z227" s="2"/>
     </row>
     <row r="228" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A228" s="8" t="s">
-        <v>602</v>
-      </c>
-      <c r="B228" s="8" t="s">
+      <c r="A228" s="6" t="s">
         <v>603</v>
       </c>
-      <c r="C228" s="33" t="s">
+      <c r="B228" s="6"/>
+      <c r="C228" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="D228" s="8" t="s">
-        <v>605</v>
+      <c r="D228" s="6" t="s">
+        <v>603</v>
       </c>
       <c r="E228" s="6"/>
       <c r="F228" s="2"/>
@@ -11268,14 +11264,16 @@
     </row>
     <row r="229" spans="1:26" ht="15.75" customHeight="1">
       <c r="A229" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B229" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="B229" s="6"/>
       <c r="C229" s="6" t="s">
         <v>607</v>
       </c>
       <c r="D229" s="6" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="E229" s="6"/>
       <c r="F229" s="2"/>
@@ -11301,50 +11299,48 @@
       <c r="Z229" s="2"/>
     </row>
     <row r="230" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A230" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="B230" s="6" t="s">
+      <c r="A230" s="12" t="s">
         <v>609</v>
       </c>
-      <c r="C230" s="6" t="s">
+      <c r="B230" s="12" t="s">
         <v>610</v>
       </c>
-      <c r="D230" s="6" t="s">
+      <c r="C230" s="13" t="s">
         <v>611</v>
       </c>
-      <c r="E230" s="6"/>
-      <c r="F230" s="2"/>
-      <c r="G230" s="2"/>
-      <c r="H230" s="2"/>
-      <c r="I230" s="2"/>
-      <c r="J230" s="2"/>
-      <c r="K230" s="2"/>
-      <c r="L230" s="2"/>
-      <c r="M230" s="2"/>
-      <c r="N230" s="2"/>
-      <c r="O230" s="2"/>
-      <c r="P230" s="2"/>
-      <c r="Q230" s="2"/>
-      <c r="R230" s="2"/>
-      <c r="S230" s="2"/>
-      <c r="T230" s="2"/>
-      <c r="U230" s="2"/>
-      <c r="V230" s="2"/>
-      <c r="W230" s="2"/>
-      <c r="X230" s="2"/>
-      <c r="Y230" s="2"/>
-      <c r="Z230" s="2"/>
+      <c r="D230" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="E230" s="12"/>
+      <c r="F230" s="5"/>
+      <c r="G230" s="5"/>
+      <c r="H230" s="5"/>
+      <c r="I230" s="5"/>
+      <c r="J230" s="5"/>
+      <c r="K230" s="5"/>
+      <c r="L230" s="5"/>
+      <c r="M230" s="5"/>
+      <c r="N230" s="5"/>
+      <c r="O230" s="5"/>
+      <c r="P230" s="5"/>
+      <c r="Q230" s="5"/>
+      <c r="R230" s="5"/>
+      <c r="S230" s="5"/>
+      <c r="T230" s="5"/>
+      <c r="U230" s="5"/>
+      <c r="V230" s="5"/>
+      <c r="W230" s="5"/>
+      <c r="X230" s="5"/>
+      <c r="Y230" s="5"/>
+      <c r="Z230" s="5"/>
     </row>
     <row r="231" spans="1:26" ht="15.75" customHeight="1">
       <c r="A231" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="B231" s="12" t="s">
+      <c r="B231" s="12"/>
+      <c r="C231" s="13" t="s">
         <v>613</v>
-      </c>
-      <c r="C231" s="13" t="s">
-        <v>614</v>
       </c>
       <c r="D231" s="12" t="s">
         <v>612</v>
@@ -11374,14 +11370,14 @@
     </row>
     <row r="232" spans="1:26" ht="15.75" customHeight="1">
       <c r="A232" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="B232" s="12"/>
+      <c r="C232" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="B232" s="12"/>
-      <c r="C232" s="13" t="s">
-        <v>616</v>
-      </c>
       <c r="D232" s="12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E232" s="12"/>
       <c r="F232" s="5"/>
@@ -11407,53 +11403,55 @@
       <c r="Z232" s="5"/>
     </row>
     <row r="233" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A233" s="12" t="s">
+      <c r="A233" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="B233" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="B233" s="12"/>
-      <c r="C233" s="14" t="s">
+      <c r="C233" s="6" t="s">
         <v>618</v>
       </c>
-      <c r="D233" s="12" t="s">
-        <v>617</v>
-      </c>
-      <c r="E233" s="12"/>
-      <c r="F233" s="5"/>
-      <c r="G233" s="5"/>
-      <c r="H233" s="5"/>
-      <c r="I233" s="5"/>
-      <c r="J233" s="5"/>
-      <c r="K233" s="5"/>
-      <c r="L233" s="5"/>
-      <c r="M233" s="5"/>
-      <c r="N233" s="5"/>
-      <c r="O233" s="5"/>
-      <c r="P233" s="5"/>
-      <c r="Q233" s="5"/>
-      <c r="R233" s="5"/>
-      <c r="S233" s="5"/>
-      <c r="T233" s="5"/>
-      <c r="U233" s="5"/>
-      <c r="V233" s="5"/>
-      <c r="W233" s="5"/>
-      <c r="X233" s="5"/>
-      <c r="Y233" s="5"/>
-      <c r="Z233" s="5"/>
+      <c r="D233" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="E233" s="6"/>
+      <c r="F233" s="2"/>
+      <c r="G233" s="2"/>
+      <c r="H233" s="2"/>
+      <c r="I233" s="2"/>
+      <c r="J233" s="2"/>
+      <c r="K233" s="2"/>
+      <c r="L233" s="2"/>
+      <c r="M233" s="2"/>
+      <c r="N233" s="2"/>
+      <c r="O233" s="2"/>
+      <c r="P233" s="2"/>
+      <c r="Q233" s="2"/>
+      <c r="R233" s="2"/>
+      <c r="S233" s="2"/>
+      <c r="T233" s="2"/>
+      <c r="U233" s="2"/>
+      <c r="V233" s="2"/>
+      <c r="W233" s="2"/>
+      <c r="X233" s="2"/>
+      <c r="Y233" s="2"/>
+      <c r="Z233" s="2"/>
     </row>
     <row r="234" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A234" s="6" t="s">
+      <c r="A234" s="10" t="s">
         <v>619</v>
       </c>
-      <c r="B234" s="6" t="s">
+      <c r="B234" s="10" t="s">
         <v>620</v>
       </c>
-      <c r="C234" s="6" t="s">
+      <c r="C234" s="32" t="s">
         <v>621</v>
       </c>
-      <c r="D234" s="6" t="s">
-        <v>619</v>
-      </c>
-      <c r="E234" s="6"/>
+      <c r="D234" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="E234" s="10"/>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
       <c r="H234" s="2"/>
@@ -11477,55 +11475,55 @@
       <c r="Z234" s="2"/>
     </row>
     <row r="235" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A235" s="10" t="s">
-        <v>622</v>
-      </c>
-      <c r="B235" s="10" t="s">
+      <c r="A235" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="C235" s="32" t="s">
+      <c r="B235" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="D235" s="10" t="s">
+      <c r="C235" s="19" t="s">
         <v>625</v>
       </c>
-      <c r="E235" s="10"/>
-      <c r="F235" s="2"/>
-      <c r="G235" s="2"/>
-      <c r="H235" s="2"/>
-      <c r="I235" s="2"/>
-      <c r="J235" s="2"/>
-      <c r="K235" s="2"/>
-      <c r="L235" s="2"/>
-      <c r="M235" s="2"/>
-      <c r="N235" s="2"/>
-      <c r="O235" s="2"/>
-      <c r="P235" s="2"/>
-      <c r="Q235" s="2"/>
-      <c r="R235" s="2"/>
-      <c r="S235" s="2"/>
-      <c r="T235" s="2"/>
-      <c r="U235" s="2"/>
-      <c r="V235" s="2"/>
-      <c r="W235" s="2"/>
-      <c r="X235" s="2"/>
-      <c r="Y235" s="2"/>
-      <c r="Z235" s="2"/>
+      <c r="D235" s="37" t="s">
+        <v>626</v>
+      </c>
+      <c r="E235" s="37"/>
+      <c r="F235" s="5"/>
+      <c r="G235" s="5"/>
+      <c r="H235" s="5"/>
+      <c r="I235" s="5"/>
+      <c r="J235" s="5"/>
+      <c r="K235" s="5"/>
+      <c r="L235" s="5"/>
+      <c r="M235" s="5"/>
+      <c r="N235" s="5"/>
+      <c r="O235" s="5"/>
+      <c r="P235" s="5"/>
+      <c r="Q235" s="5"/>
+      <c r="R235" s="5"/>
+      <c r="S235" s="5"/>
+      <c r="T235" s="5"/>
+      <c r="U235" s="5"/>
+      <c r="V235" s="5"/>
+      <c r="W235" s="5"/>
+      <c r="X235" s="5"/>
+      <c r="Y235" s="5"/>
+      <c r="Z235" s="5"/>
     </row>
     <row r="236" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A236" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="B236" s="12" t="s">
+      <c r="A236" s="16" t="s">
         <v>627</v>
       </c>
-      <c r="C236" s="19" t="s">
+      <c r="B236" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="C236" s="46" t="s">
         <v>628</v>
       </c>
-      <c r="D236" s="37" t="s">
-        <v>629</v>
-      </c>
-      <c r="E236" s="37"/>
+      <c r="D236" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="E236" s="16"/>
       <c r="F236" s="5"/>
       <c r="G236" s="5"/>
       <c r="H236" s="5"/>
@@ -11550,16 +11548,14 @@
     </row>
     <row r="237" spans="1:26" ht="15.75" customHeight="1">
       <c r="A237" s="16" t="s">
+        <v>629</v>
+      </c>
+      <c r="B237" s="16"/>
+      <c r="C237" s="46" t="s">
         <v>630</v>
       </c>
-      <c r="B237" s="16" t="s">
-        <v>630</v>
-      </c>
-      <c r="C237" s="46" t="s">
-        <v>631</v>
-      </c>
       <c r="D237" s="16" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E237" s="16"/>
       <c r="F237" s="5"/>
@@ -11585,17 +11581,17 @@
       <c r="Z237" s="5"/>
     </row>
     <row r="238" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A238" s="16" t="s">
+      <c r="A238" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="B238" s="12"/>
+      <c r="C238" s="37" t="s">
         <v>632</v>
       </c>
-      <c r="B238" s="16"/>
-      <c r="C238" s="46" t="s">
-        <v>633</v>
-      </c>
-      <c r="D238" s="16" t="s">
-        <v>632</v>
-      </c>
-      <c r="E238" s="16"/>
+      <c r="D238" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="E238" s="12"/>
       <c r="F238" s="5"/>
       <c r="G238" s="5"/>
       <c r="H238" s="5"/>
@@ -11619,51 +11615,51 @@
       <c r="Z238" s="5"/>
     </row>
     <row r="239" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A239" s="12" t="s">
+      <c r="A239" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="B239" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="B239" s="12"/>
-      <c r="C239" s="37" t="s">
+      <c r="C239" s="6" t="s">
         <v>635</v>
       </c>
-      <c r="D239" s="12" t="s">
-        <v>634</v>
-      </c>
-      <c r="E239" s="12"/>
-      <c r="F239" s="5"/>
-      <c r="G239" s="5"/>
-      <c r="H239" s="5"/>
-      <c r="I239" s="5"/>
-      <c r="J239" s="5"/>
-      <c r="K239" s="5"/>
-      <c r="L239" s="5"/>
-      <c r="M239" s="5"/>
-      <c r="N239" s="5"/>
-      <c r="O239" s="5"/>
-      <c r="P239" s="5"/>
-      <c r="Q239" s="5"/>
-      <c r="R239" s="5"/>
-      <c r="S239" s="5"/>
-      <c r="T239" s="5"/>
-      <c r="U239" s="5"/>
-      <c r="V239" s="5"/>
-      <c r="W239" s="5"/>
-      <c r="X239" s="5"/>
-      <c r="Y239" s="5"/>
-      <c r="Z239" s="5"/>
+      <c r="D239" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="E239" s="6"/>
+      <c r="F239" s="2"/>
+      <c r="G239" s="2"/>
+      <c r="H239" s="2"/>
+      <c r="I239" s="2"/>
+      <c r="J239" s="2"/>
+      <c r="K239" s="2"/>
+      <c r="L239" s="2"/>
+      <c r="M239" s="2"/>
+      <c r="N239" s="2"/>
+      <c r="O239" s="2"/>
+      <c r="P239" s="2"/>
+      <c r="Q239" s="2"/>
+      <c r="R239" s="2"/>
+      <c r="S239" s="2"/>
+      <c r="T239" s="2"/>
+      <c r="U239" s="2"/>
+      <c r="V239" s="2"/>
+      <c r="W239" s="2"/>
+      <c r="X239" s="2"/>
+      <c r="Y239" s="2"/>
+      <c r="Z239" s="2"/>
     </row>
     <row r="240" spans="1:26" ht="15.75" customHeight="1">
       <c r="A240" s="6" t="s">
         <v>636</v>
       </c>
-      <c r="B240" s="6" t="s">
+      <c r="B240" s="6"/>
+      <c r="C240" s="21" t="s">
         <v>637</v>
       </c>
-      <c r="C240" s="6" t="s">
+      <c r="D240" s="6" t="s">
         <v>638</v>
-      </c>
-      <c r="D240" s="6" t="s">
-        <v>636</v>
       </c>
       <c r="E240" s="6"/>
       <c r="F240" s="2"/>
@@ -11689,47 +11685,51 @@
       <c r="Z240" s="2"/>
     </row>
     <row r="241" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A241" s="6" t="s">
+      <c r="A241" s="12" t="s">
         <v>639</v>
       </c>
-      <c r="B241" s="6"/>
-      <c r="C241" s="21" t="s">
+      <c r="B241" s="12" t="s">
         <v>640</v>
       </c>
-      <c r="D241" s="6" t="s">
+      <c r="C241" s="14" t="s">
         <v>641</v>
       </c>
-      <c r="E241" s="6"/>
-      <c r="F241" s="2"/>
-      <c r="G241" s="2"/>
-      <c r="H241" s="2"/>
-      <c r="I241" s="2"/>
-      <c r="J241" s="2"/>
-      <c r="K241" s="2"/>
-      <c r="L241" s="2"/>
-      <c r="M241" s="2"/>
-      <c r="N241" s="2"/>
-      <c r="O241" s="2"/>
-      <c r="P241" s="2"/>
-      <c r="Q241" s="2"/>
-      <c r="R241" s="2"/>
-      <c r="S241" s="2"/>
-      <c r="T241" s="2"/>
-      <c r="U241" s="2"/>
-      <c r="V241" s="2"/>
-      <c r="W241" s="2"/>
-      <c r="X241" s="2"/>
-      <c r="Y241" s="2"/>
-      <c r="Z241" s="2"/>
+      <c r="D241" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="E241" s="12"/>
+      <c r="F241" s="5"/>
+      <c r="G241" s="5"/>
+      <c r="H241" s="5"/>
+      <c r="I241" s="5"/>
+      <c r="J241" s="5"/>
+      <c r="K241" s="5"/>
+      <c r="L241" s="5"/>
+      <c r="M241" s="5"/>
+      <c r="N241" s="5"/>
+      <c r="O241" s="5"/>
+      <c r="P241" s="5"/>
+      <c r="Q241" s="5"/>
+      <c r="R241" s="5"/>
+      <c r="S241" s="5"/>
+      <c r="T241" s="5"/>
+      <c r="U241" s="5"/>
+      <c r="V241" s="5"/>
+      <c r="W241" s="5"/>
+      <c r="X241" s="5"/>
+      <c r="Y241" s="5"/>
+      <c r="Z241" s="5"/>
     </row>
     <row r="242" spans="1:26" ht="15.75" customHeight="1">
       <c r="A242" s="12" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B242" s="12"/>
-      <c r="C242" s="13"/>
+      <c r="C242" s="13" t="s">
+        <v>644</v>
+      </c>
       <c r="D242" s="12" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="E242" s="12"/>
       <c r="F242" s="5"/>
@@ -11755,17 +11755,17 @@
       <c r="Z242" s="5"/>
     </row>
     <row r="243" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A243" s="12" t="s">
-        <v>644</v>
-      </c>
-      <c r="B243" s="12" t="s">
-        <v>645</v>
-      </c>
-      <c r="C243" s="14" t="s">
+      <c r="A243" s="16" t="s">
         <v>646</v>
       </c>
-      <c r="D243" s="12" t="s">
+      <c r="B243" s="16" t="s">
         <v>647</v>
+      </c>
+      <c r="C243" s="17" t="s">
+        <v>648</v>
+      </c>
+      <c r="D243" s="16" t="s">
+        <v>646</v>
       </c>
       <c r="E243" s="12"/>
       <c r="F243" s="5"/>
@@ -11792,14 +11792,14 @@
     </row>
     <row r="244" spans="1:26" ht="15.75" customHeight="1">
       <c r="A244" s="12" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B244" s="12"/>
       <c r="C244" s="13" t="s">
+        <v>650</v>
+      </c>
+      <c r="D244" s="12" t="s">
         <v>649</v>
-      </c>
-      <c r="D244" s="12" t="s">
-        <v>650</v>
       </c>
       <c r="E244" s="12"/>
       <c r="F244" s="5"/>
@@ -11825,16 +11825,14 @@
       <c r="Z244" s="5"/>
     </row>
     <row r="245" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A245" s="16" t="s">
+      <c r="A245" s="12" t="s">
         <v>651</v>
       </c>
-      <c r="B245" s="16" t="s">
+      <c r="B245" s="12"/>
+      <c r="C245" s="14" t="s">
         <v>652</v>
       </c>
-      <c r="C245" s="17" t="s">
-        <v>653</v>
-      </c>
-      <c r="D245" s="16" t="s">
+      <c r="D245" s="12" t="s">
         <v>651</v>
       </c>
       <c r="E245" s="12"/>
@@ -11862,14 +11860,14 @@
     </row>
     <row r="246" spans="1:26" ht="15.75" customHeight="1">
       <c r="A246" s="12" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B246" s="12"/>
       <c r="C246" s="13" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D246" s="12" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E246" s="12"/>
       <c r="F246" s="5"/>
@@ -11896,14 +11894,16 @@
     </row>
     <row r="247" spans="1:26" ht="15.75" customHeight="1">
       <c r="A247" s="12" t="s">
+        <v>655</v>
+      </c>
+      <c r="B247" s="12" t="s">
         <v>656</v>
       </c>
-      <c r="B247" s="12"/>
       <c r="C247" s="14" t="s">
         <v>657</v>
       </c>
       <c r="D247" s="12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E247" s="12"/>
       <c r="F247" s="5"/>
@@ -11933,7 +11933,7 @@
         <v>658</v>
       </c>
       <c r="B248" s="12"/>
-      <c r="C248" s="13" t="s">
+      <c r="C248" s="19" t="s">
         <v>659</v>
       </c>
       <c r="D248" s="12" t="s">
@@ -11966,11 +11966,9 @@
       <c r="A249" s="12" t="s">
         <v>660</v>
       </c>
-      <c r="B249" s="12" t="s">
+      <c r="B249" s="12"/>
+      <c r="C249" s="13" t="s">
         <v>661</v>
-      </c>
-      <c r="C249" s="14" t="s">
-        <v>662</v>
       </c>
       <c r="D249" s="12" t="s">
         <v>660</v>
@@ -11999,87 +11997,87 @@
       <c r="Z249" s="5"/>
     </row>
     <row r="250" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A250" s="12" t="s">
+      <c r="A250" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="B250" s="8" t="s">
         <v>663</v>
       </c>
-      <c r="B250" s="12"/>
-      <c r="C250" s="19" t="s">
+      <c r="C250" s="33" t="s">
         <v>664</v>
       </c>
-      <c r="D250" s="12" t="s">
-        <v>663</v>
-      </c>
-      <c r="E250" s="12"/>
-      <c r="F250" s="5"/>
-      <c r="G250" s="5"/>
-      <c r="H250" s="5"/>
-      <c r="I250" s="5"/>
-      <c r="J250" s="5"/>
-      <c r="K250" s="5"/>
-      <c r="L250" s="5"/>
-      <c r="M250" s="5"/>
-      <c r="N250" s="5"/>
-      <c r="O250" s="5"/>
-      <c r="P250" s="5"/>
-      <c r="Q250" s="5"/>
-      <c r="R250" s="5"/>
-      <c r="S250" s="5"/>
-      <c r="T250" s="5"/>
-      <c r="U250" s="5"/>
-      <c r="V250" s="5"/>
-      <c r="W250" s="5"/>
-      <c r="X250" s="5"/>
-      <c r="Y250" s="5"/>
-      <c r="Z250" s="5"/>
+      <c r="D250" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="E250" s="8"/>
+      <c r="F250" s="2"/>
+      <c r="G250" s="2"/>
+      <c r="H250" s="2"/>
+      <c r="I250" s="2"/>
+      <c r="J250" s="2"/>
+      <c r="K250" s="2"/>
+      <c r="L250" s="2"/>
+      <c r="M250" s="2"/>
+      <c r="N250" s="2"/>
+      <c r="O250" s="2"/>
+      <c r="P250" s="2"/>
+      <c r="Q250" s="2"/>
+      <c r="R250" s="2"/>
+      <c r="S250" s="2"/>
+      <c r="T250" s="2"/>
+      <c r="U250" s="2"/>
+      <c r="V250" s="2"/>
+      <c r="W250" s="2"/>
+      <c r="X250" s="2"/>
+      <c r="Y250" s="2"/>
+      <c r="Z250" s="2"/>
     </row>
     <row r="251" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A251" s="12" t="s">
+      <c r="A251" s="6" t="s">
         <v>665</v>
       </c>
-      <c r="B251" s="12"/>
-      <c r="C251" s="13" t="s">
+      <c r="B251" s="6"/>
+      <c r="C251" s="6" t="s">
         <v>666</v>
       </c>
-      <c r="D251" s="12" t="s">
-        <v>665</v>
-      </c>
-      <c r="E251" s="12"/>
-      <c r="F251" s="5"/>
-      <c r="G251" s="5"/>
-      <c r="H251" s="5"/>
-      <c r="I251" s="5"/>
-      <c r="J251" s="5"/>
-      <c r="K251" s="5"/>
-      <c r="L251" s="5"/>
-      <c r="M251" s="5"/>
-      <c r="N251" s="5"/>
-      <c r="O251" s="5"/>
-      <c r="P251" s="5"/>
-      <c r="Q251" s="5"/>
-      <c r="R251" s="5"/>
-      <c r="S251" s="5"/>
-      <c r="T251" s="5"/>
-      <c r="U251" s="5"/>
-      <c r="V251" s="5"/>
-      <c r="W251" s="5"/>
-      <c r="X251" s="5"/>
-      <c r="Y251" s="5"/>
-      <c r="Z251" s="5"/>
+      <c r="D251" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="E251" s="6"/>
+      <c r="F251" s="2"/>
+      <c r="G251" s="2"/>
+      <c r="H251" s="2"/>
+      <c r="I251" s="2"/>
+      <c r="J251" s="2"/>
+      <c r="K251" s="2"/>
+      <c r="L251" s="2"/>
+      <c r="M251" s="2"/>
+      <c r="N251" s="2"/>
+      <c r="O251" s="2"/>
+      <c r="P251" s="2"/>
+      <c r="Q251" s="2"/>
+      <c r="R251" s="2"/>
+      <c r="S251" s="2"/>
+      <c r="T251" s="2"/>
+      <c r="U251" s="2"/>
+      <c r="V251" s="2"/>
+      <c r="W251" s="2"/>
+      <c r="X251" s="2"/>
+      <c r="Y251" s="2"/>
+      <c r="Z251" s="2"/>
     </row>
     <row r="252" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A252" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="B252" s="8" t="s">
+      <c r="A252" s="6" t="s">
         <v>668</v>
       </c>
-      <c r="C252" s="33" t="s">
+      <c r="B252" s="6"/>
+      <c r="C252" s="6" t="s">
         <v>669</v>
       </c>
-      <c r="D252" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="E252" s="8"/>
+      <c r="D252" s="6" t="s">
+        <v>668</v>
+      </c>
+      <c r="E252" s="6"/>
       <c r="F252" s="2"/>
       <c r="G252" s="2"/>
       <c r="H252" s="2"/>
@@ -12103,15 +12101,17 @@
       <c r="Z252" s="2"/>
     </row>
     <row r="253" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A253" s="6" t="s">
+      <c r="A253" s="10" t="s">
         <v>670</v>
       </c>
-      <c r="B253" s="6"/>
-      <c r="C253" s="6" t="s">
+      <c r="B253" s="10" t="s">
         <v>671</v>
       </c>
-      <c r="D253" s="6" t="s">
+      <c r="C253" s="11" t="s">
         <v>672</v>
+      </c>
+      <c r="D253" s="10" t="s">
+        <v>670</v>
       </c>
       <c r="E253" s="6"/>
       <c r="F253" s="2"/>
@@ -12137,85 +12137,87 @@
       <c r="Z253" s="2"/>
     </row>
     <row r="254" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A254" s="6" t="s">
+      <c r="A254" s="12" t="s">
         <v>673</v>
       </c>
-      <c r="B254" s="6"/>
-      <c r="C254" s="6" t="s">
+      <c r="B254" s="12"/>
+      <c r="C254" s="14" t="s">
         <v>674</v>
       </c>
-      <c r="D254" s="6" t="s">
+      <c r="D254" s="12" t="s">
         <v>673</v>
       </c>
-      <c r="E254" s="6"/>
-      <c r="F254" s="2"/>
-      <c r="G254" s="2"/>
-      <c r="H254" s="2"/>
-      <c r="I254" s="2"/>
-      <c r="J254" s="2"/>
-      <c r="K254" s="2"/>
-      <c r="L254" s="2"/>
-      <c r="M254" s="2"/>
-      <c r="N254" s="2"/>
-      <c r="O254" s="2"/>
-      <c r="P254" s="2"/>
-      <c r="Q254" s="2"/>
-      <c r="R254" s="2"/>
-      <c r="S254" s="2"/>
-      <c r="T254" s="2"/>
-      <c r="U254" s="2"/>
-      <c r="V254" s="2"/>
-      <c r="W254" s="2"/>
-      <c r="X254" s="2"/>
-      <c r="Y254" s="2"/>
-      <c r="Z254" s="2"/>
+      <c r="E254" s="12"/>
+      <c r="F254" s="5"/>
+      <c r="G254" s="5"/>
+      <c r="H254" s="5"/>
+      <c r="I254" s="5"/>
+      <c r="J254" s="5"/>
+      <c r="K254" s="5"/>
+      <c r="L254" s="5"/>
+      <c r="M254" s="5"/>
+      <c r="N254" s="5"/>
+      <c r="O254" s="5"/>
+      <c r="P254" s="5"/>
+      <c r="Q254" s="5"/>
+      <c r="R254" s="5"/>
+      <c r="S254" s="5"/>
+      <c r="T254" s="5"/>
+      <c r="U254" s="5"/>
+      <c r="V254" s="5"/>
+      <c r="W254" s="5"/>
+      <c r="X254" s="5"/>
+      <c r="Y254" s="5"/>
+      <c r="Z254" s="5"/>
     </row>
     <row r="255" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A255" s="10" t="s">
+      <c r="A255" s="12" t="s">
         <v>675</v>
       </c>
-      <c r="B255" s="10" t="s">
+      <c r="B255" s="12" t="s">
         <v>676</v>
       </c>
-      <c r="C255" s="11" t="s">
+      <c r="C255" s="51" t="s">
         <v>677</v>
       </c>
-      <c r="D255" s="10" t="s">
-        <v>675</v>
-      </c>
-      <c r="E255" s="6"/>
-      <c r="F255" s="2"/>
-      <c r="G255" s="2"/>
-      <c r="H255" s="2"/>
-      <c r="I255" s="2"/>
-      <c r="J255" s="2"/>
-      <c r="K255" s="2"/>
-      <c r="L255" s="2"/>
-      <c r="M255" s="2"/>
-      <c r="N255" s="2"/>
-      <c r="O255" s="2"/>
-      <c r="P255" s="2"/>
-      <c r="Q255" s="2"/>
-      <c r="R255" s="2"/>
-      <c r="S255" s="2"/>
-      <c r="T255" s="2"/>
-      <c r="U255" s="2"/>
-      <c r="V255" s="2"/>
-      <c r="W255" s="2"/>
-      <c r="X255" s="2"/>
-      <c r="Y255" s="2"/>
-      <c r="Z255" s="2"/>
+      <c r="D255" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="E255" s="12"/>
+      <c r="F255" s="5"/>
+      <c r="G255" s="5"/>
+      <c r="H255" s="5"/>
+      <c r="I255" s="5"/>
+      <c r="J255" s="5"/>
+      <c r="K255" s="5"/>
+      <c r="L255" s="5"/>
+      <c r="M255" s="5"/>
+      <c r="N255" s="5"/>
+      <c r="O255" s="5"/>
+      <c r="P255" s="5"/>
+      <c r="Q255" s="5"/>
+      <c r="R255" s="5"/>
+      <c r="S255" s="5"/>
+      <c r="T255" s="5"/>
+      <c r="U255" s="5"/>
+      <c r="V255" s="5"/>
+      <c r="W255" s="5"/>
+      <c r="X255" s="5"/>
+      <c r="Y255" s="5"/>
+      <c r="Z255" s="5"/>
     </row>
     <row r="256" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A256" s="12" t="s">
-        <v>678</v>
-      </c>
-      <c r="B256" s="12"/>
-      <c r="C256" s="14" t="s">
+      <c r="A256" s="16" t="s">
         <v>679</v>
       </c>
-      <c r="D256" s="12" t="s">
-        <v>678</v>
+      <c r="B256" s="16" t="s">
+        <v>680</v>
+      </c>
+      <c r="C256" s="52" t="s">
+        <v>681</v>
+      </c>
+      <c r="D256" s="16" t="s">
+        <v>682</v>
       </c>
       <c r="E256" s="12"/>
       <c r="F256" s="5"/>
@@ -12242,16 +12244,16 @@
     </row>
     <row r="257" spans="1:26" ht="15.75" customHeight="1">
       <c r="A257" s="12" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>681</v>
-      </c>
-      <c r="C257" s="51" t="s">
-        <v>682</v>
+        <v>684</v>
+      </c>
+      <c r="C257" s="13" t="s">
+        <v>685</v>
       </c>
       <c r="D257" s="12" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="E257" s="12"/>
       <c r="F257" s="5"/>
@@ -12278,16 +12280,14 @@
     </row>
     <row r="258" spans="1:26" ht="15.75" customHeight="1">
       <c r="A258" s="16" t="s">
-        <v>684</v>
-      </c>
-      <c r="B258" s="16" t="s">
-        <v>685</v>
-      </c>
-      <c r="C258" s="52" t="s">
-        <v>686</v>
+        <v>687</v>
+      </c>
+      <c r="B258" s="16"/>
+      <c r="C258" s="17" t="s">
+        <v>688</v>
       </c>
       <c r="D258" s="16" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="E258" s="12"/>
       <c r="F258" s="5"/>
@@ -12314,18 +12314,16 @@
     </row>
     <row r="259" spans="1:26" ht="15.75" customHeight="1">
       <c r="A259" s="12" t="s">
-        <v>688</v>
-      </c>
-      <c r="B259" s="12" t="s">
-        <v>689</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="B259" s="12"/>
       <c r="C259" s="13" t="s">
+        <v>691</v>
+      </c>
+      <c r="D259" s="12" t="s">
         <v>690</v>
       </c>
-      <c r="D259" s="12" t="s">
-        <v>691</v>
-      </c>
-      <c r="E259" s="12"/>
+      <c r="E259" s="16"/>
       <c r="F259" s="5"/>
       <c r="G259" s="5"/>
       <c r="H259" s="5"/>
@@ -12349,17 +12347,19 @@
       <c r="Z259" s="5"/>
     </row>
     <row r="260" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A260" s="16" t="s">
+      <c r="A260" s="12" t="s">
         <v>692</v>
       </c>
-      <c r="B260" s="16"/>
-      <c r="C260" s="17" t="s">
+      <c r="B260" s="12" t="s">
         <v>693</v>
       </c>
-      <c r="D260" s="16" t="s">
+      <c r="C260" s="14" t="s">
         <v>694</v>
       </c>
-      <c r="E260" s="12"/>
+      <c r="D260" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="E260" s="16"/>
       <c r="F260" s="5"/>
       <c r="G260" s="5"/>
       <c r="H260" s="5"/>
@@ -12384,14 +12384,14 @@
     </row>
     <row r="261" spans="1:26" ht="15.75" customHeight="1">
       <c r="A261" s="12" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B261" s="12"/>
       <c r="C261" s="13" t="s">
-        <v>696</v>
+        <v>846</v>
       </c>
       <c r="D261" s="12" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E261" s="16"/>
       <c r="F261" s="5"/>
@@ -12417,17 +12417,15 @@
       <c r="Z261" s="5"/>
     </row>
     <row r="262" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A262" s="12" t="s">
-        <v>697</v>
-      </c>
-      <c r="B262" s="12" t="s">
+      <c r="A262" s="16" t="s">
         <v>698</v>
       </c>
-      <c r="C262" s="14" t="s">
+      <c r="B262" s="16"/>
+      <c r="C262" s="25" t="s">
         <v>699</v>
       </c>
-      <c r="D262" s="12" t="s">
-        <v>700</v>
+      <c r="D262" s="16" t="s">
+        <v>698</v>
       </c>
       <c r="E262" s="16"/>
       <c r="F262" s="5"/>
@@ -12453,15 +12451,17 @@
       <c r="Z262" s="5"/>
     </row>
     <row r="263" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A263" s="12" t="s">
+      <c r="A263" s="16" t="s">
+        <v>700</v>
+      </c>
+      <c r="B263" s="16" t="s">
         <v>701</v>
       </c>
-      <c r="B263" s="12"/>
-      <c r="C263" s="13" t="s">
-        <v>851</v>
-      </c>
-      <c r="D263" s="12" t="s">
+      <c r="C263" s="17" t="s">
         <v>702</v>
+      </c>
+      <c r="D263" s="16" t="s">
+        <v>700</v>
       </c>
       <c r="E263" s="16"/>
       <c r="F263" s="5"/>
@@ -12487,17 +12487,19 @@
       <c r="Z263" s="5"/>
     </row>
     <row r="264" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A264" s="16" t="s">
+      <c r="A264" s="12" t="s">
         <v>703</v>
       </c>
-      <c r="B264" s="16"/>
-      <c r="C264" s="25" t="s">
+      <c r="B264" s="12" t="s">
         <v>704</v>
       </c>
-      <c r="D264" s="16" t="s">
+      <c r="C264" s="13" t="s">
+        <v>705</v>
+      </c>
+      <c r="D264" s="12" t="s">
         <v>703</v>
       </c>
-      <c r="E264" s="16"/>
+      <c r="E264" s="12"/>
       <c r="F264" s="5"/>
       <c r="G264" s="5"/>
       <c r="H264" s="5"/>
@@ -12521,19 +12523,19 @@
       <c r="Z264" s="5"/>
     </row>
     <row r="265" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A265" s="16" t="s">
-        <v>705</v>
-      </c>
-      <c r="B265" s="16" t="s">
+      <c r="A265" s="12" t="s">
         <v>706</v>
       </c>
-      <c r="C265" s="17" t="s">
+      <c r="B265" s="12" t="s">
         <v>707</v>
       </c>
-      <c r="D265" s="16" t="s">
-        <v>705</v>
-      </c>
-      <c r="E265" s="16"/>
+      <c r="C265" s="13" t="s">
+        <v>708</v>
+      </c>
+      <c r="D265" s="12" t="s">
+        <v>706</v>
+      </c>
+      <c r="E265" s="12"/>
       <c r="F265" s="5"/>
       <c r="G265" s="5"/>
       <c r="H265" s="5"/>
@@ -12557,91 +12559,91 @@
       <c r="Z265" s="5"/>
     </row>
     <row r="266" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A266" s="12" t="s">
-        <v>708</v>
-      </c>
-      <c r="B266" s="12" t="s">
+      <c r="A266" s="6" t="s">
         <v>709</v>
       </c>
-      <c r="C266" s="13" t="s">
+      <c r="B266" s="6" t="s">
         <v>710</v>
       </c>
-      <c r="D266" s="12" t="s">
-        <v>708</v>
-      </c>
-      <c r="E266" s="12"/>
-      <c r="F266" s="5"/>
-      <c r="G266" s="5"/>
-      <c r="H266" s="5"/>
-      <c r="I266" s="5"/>
-      <c r="J266" s="5"/>
-      <c r="K266" s="5"/>
-      <c r="L266" s="5"/>
-      <c r="M266" s="5"/>
-      <c r="N266" s="5"/>
-      <c r="O266" s="5"/>
-      <c r="P266" s="5"/>
-      <c r="Q266" s="5"/>
-      <c r="R266" s="5"/>
-      <c r="S266" s="5"/>
-      <c r="T266" s="5"/>
-      <c r="U266" s="5"/>
-      <c r="V266" s="5"/>
-      <c r="W266" s="5"/>
-      <c r="X266" s="5"/>
-      <c r="Y266" s="5"/>
-      <c r="Z266" s="5"/>
+      <c r="C266" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="D266" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="E266" s="6"/>
+      <c r="F266" s="2"/>
+      <c r="G266" s="2"/>
+      <c r="H266" s="2"/>
+      <c r="I266" s="2"/>
+      <c r="J266" s="2"/>
+      <c r="K266" s="2"/>
+      <c r="L266" s="2"/>
+      <c r="M266" s="2"/>
+      <c r="N266" s="2"/>
+      <c r="O266" s="2"/>
+      <c r="P266" s="2"/>
+      <c r="Q266" s="2"/>
+      <c r="R266" s="2"/>
+      <c r="S266" s="2"/>
+      <c r="T266" s="2"/>
+      <c r="U266" s="2"/>
+      <c r="V266" s="2"/>
+      <c r="W266" s="2"/>
+      <c r="X266" s="2"/>
+      <c r="Y266" s="2"/>
+      <c r="Z266" s="2"/>
     </row>
     <row r="267" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A267" s="12" t="s">
-        <v>711</v>
-      </c>
-      <c r="B267" s="12" t="s">
+      <c r="A267" s="6" t="s">
         <v>712</v>
       </c>
-      <c r="C267" s="13" t="s">
+      <c r="B267" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="D267" s="12" t="s">
-        <v>711</v>
-      </c>
-      <c r="E267" s="12"/>
-      <c r="F267" s="5"/>
-      <c r="G267" s="5"/>
-      <c r="H267" s="5"/>
-      <c r="I267" s="5"/>
-      <c r="J267" s="5"/>
-      <c r="K267" s="5"/>
-      <c r="L267" s="5"/>
-      <c r="M267" s="5"/>
-      <c r="N267" s="5"/>
-      <c r="O267" s="5"/>
-      <c r="P267" s="5"/>
-      <c r="Q267" s="5"/>
-      <c r="R267" s="5"/>
-      <c r="S267" s="5"/>
-      <c r="T267" s="5"/>
-      <c r="U267" s="5"/>
-      <c r="V267" s="5"/>
-      <c r="W267" s="5"/>
-      <c r="X267" s="5"/>
-      <c r="Y267" s="5"/>
-      <c r="Z267" s="5"/>
+      <c r="C267" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="D267" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="E267" s="6"/>
+      <c r="F267" s="2"/>
+      <c r="G267" s="2"/>
+      <c r="H267" s="2"/>
+      <c r="I267" s="2"/>
+      <c r="J267" s="2"/>
+      <c r="K267" s="2"/>
+      <c r="L267" s="2"/>
+      <c r="M267" s="2"/>
+      <c r="N267" s="2"/>
+      <c r="O267" s="2"/>
+      <c r="P267" s="2"/>
+      <c r="Q267" s="2"/>
+      <c r="R267" s="2"/>
+      <c r="S267" s="2"/>
+      <c r="T267" s="2"/>
+      <c r="U267" s="2"/>
+      <c r="V267" s="2"/>
+      <c r="W267" s="2"/>
+      <c r="X267" s="2"/>
+      <c r="Y267" s="2"/>
+      <c r="Z267" s="2"/>
     </row>
     <row r="268" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A268" s="6" t="s">
-        <v>714</v>
-      </c>
-      <c r="B268" s="6" t="s">
+      <c r="A268" s="8" t="s">
         <v>715</v>
       </c>
-      <c r="C268" s="6" t="s">
+      <c r="B268" s="8" t="s">
         <v>716</v>
       </c>
-      <c r="D268" s="6" t="s">
-        <v>714</v>
-      </c>
-      <c r="E268" s="6"/>
+      <c r="C268" s="53" t="s">
+        <v>717</v>
+      </c>
+      <c r="D268" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="E268" s="8"/>
       <c r="F268" s="2"/>
       <c r="G268" s="2"/>
       <c r="H268" s="2"/>
@@ -12665,19 +12667,17 @@
       <c r="Z268" s="2"/>
     </row>
     <row r="269" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A269" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="B269" s="6" t="s">
-        <v>718</v>
-      </c>
-      <c r="C269" s="7" t="s">
+      <c r="A269" s="8" t="s">
         <v>719</v>
       </c>
-      <c r="D269" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="E269" s="6"/>
+      <c r="B269" s="8"/>
+      <c r="C269" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="D269" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="E269" s="8"/>
       <c r="F269" s="2"/>
       <c r="G269" s="2"/>
       <c r="H269" s="2"/>
@@ -12701,19 +12701,19 @@
       <c r="Z269" s="2"/>
     </row>
     <row r="270" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A270" s="8" t="s">
-        <v>720</v>
-      </c>
-      <c r="B270" s="8" t="s">
+      <c r="A270" s="6" t="s">
         <v>721</v>
       </c>
-      <c r="C270" s="53" t="s">
+      <c r="B270" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="D270" s="8" t="s">
+      <c r="C270" s="6" t="s">
         <v>723</v>
       </c>
-      <c r="E270" s="8"/>
+      <c r="D270" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="E270" s="6"/>
       <c r="F270" s="2"/>
       <c r="G270" s="2"/>
       <c r="H270" s="2"/>
@@ -12737,51 +12737,53 @@
       <c r="Z270" s="2"/>
     </row>
     <row r="271" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A271" s="8" t="s">
+      <c r="A271" s="12" t="s">
         <v>724</v>
       </c>
-      <c r="B271" s="8"/>
-      <c r="C271" s="9" t="s">
+      <c r="B271" s="12" t="s">
         <v>725</v>
       </c>
-      <c r="D271" s="8" t="s">
+      <c r="C271" s="14" t="s">
+        <v>726</v>
+      </c>
+      <c r="D271" s="12" t="s">
         <v>724</v>
       </c>
-      <c r="E271" s="8"/>
-      <c r="F271" s="2"/>
-      <c r="G271" s="2"/>
-      <c r="H271" s="2"/>
-      <c r="I271" s="2"/>
-      <c r="J271" s="2"/>
-      <c r="K271" s="2"/>
-      <c r="L271" s="2"/>
-      <c r="M271" s="2"/>
-      <c r="N271" s="2"/>
-      <c r="O271" s="2"/>
-      <c r="P271" s="2"/>
-      <c r="Q271" s="2"/>
-      <c r="R271" s="2"/>
-      <c r="S271" s="2"/>
-      <c r="T271" s="2"/>
-      <c r="U271" s="2"/>
-      <c r="V271" s="2"/>
-      <c r="W271" s="2"/>
-      <c r="X271" s="2"/>
-      <c r="Y271" s="2"/>
-      <c r="Z271" s="2"/>
+      <c r="E271" s="12"/>
+      <c r="F271" s="5"/>
+      <c r="G271" s="5"/>
+      <c r="H271" s="5"/>
+      <c r="I271" s="5"/>
+      <c r="J271" s="5"/>
+      <c r="K271" s="5"/>
+      <c r="L271" s="5"/>
+      <c r="M271" s="5"/>
+      <c r="N271" s="5"/>
+      <c r="O271" s="5"/>
+      <c r="P271" s="5"/>
+      <c r="Q271" s="5"/>
+      <c r="R271" s="5"/>
+      <c r="S271" s="5"/>
+      <c r="T271" s="5"/>
+      <c r="U271" s="5"/>
+      <c r="V271" s="5"/>
+      <c r="W271" s="5"/>
+      <c r="X271" s="5"/>
+      <c r="Y271" s="5"/>
+      <c r="Z271" s="5"/>
     </row>
     <row r="272" spans="1:26" ht="15.75" customHeight="1">
       <c r="A272" s="6" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B272" s="6" t="s">
-        <v>727</v>
-      </c>
-      <c r="C272" s="6" t="s">
         <v>728</v>
       </c>
+      <c r="C272" s="7" t="s">
+        <v>847</v>
+      </c>
       <c r="D272" s="6" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="E272" s="6"/>
       <c r="F272" s="2"/>
@@ -12807,53 +12809,49 @@
       <c r="Z272" s="2"/>
     </row>
     <row r="273" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A273" s="12" t="s">
-        <v>729</v>
-      </c>
-      <c r="B273" s="12" t="s">
+      <c r="A273" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="C273" s="14" t="s">
+      <c r="B273" s="8"/>
+      <c r="C273" s="53" t="s">
         <v>731</v>
       </c>
-      <c r="D273" s="12" t="s">
-        <v>729</v>
-      </c>
-      <c r="E273" s="12"/>
-      <c r="F273" s="5"/>
-      <c r="G273" s="5"/>
-      <c r="H273" s="5"/>
-      <c r="I273" s="5"/>
-      <c r="J273" s="5"/>
-      <c r="K273" s="5"/>
-      <c r="L273" s="5"/>
-      <c r="M273" s="5"/>
-      <c r="N273" s="5"/>
-      <c r="O273" s="5"/>
-      <c r="P273" s="5"/>
-      <c r="Q273" s="5"/>
-      <c r="R273" s="5"/>
-      <c r="S273" s="5"/>
-      <c r="T273" s="5"/>
-      <c r="U273" s="5"/>
-      <c r="V273" s="5"/>
-      <c r="W273" s="5"/>
-      <c r="X273" s="5"/>
-      <c r="Y273" s="5"/>
-      <c r="Z273" s="5"/>
+      <c r="D273" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="E273" s="6"/>
+      <c r="F273" s="2"/>
+      <c r="G273" s="2"/>
+      <c r="H273" s="2"/>
+      <c r="I273" s="2"/>
+      <c r="J273" s="2"/>
+      <c r="K273" s="2"/>
+      <c r="L273" s="2"/>
+      <c r="M273" s="2"/>
+      <c r="N273" s="2"/>
+      <c r="O273" s="2"/>
+      <c r="P273" s="2"/>
+      <c r="Q273" s="2"/>
+      <c r="R273" s="2"/>
+      <c r="S273" s="2"/>
+      <c r="T273" s="2"/>
+      <c r="U273" s="2"/>
+      <c r="V273" s="2"/>
+      <c r="W273" s="2"/>
+      <c r="X273" s="2"/>
+      <c r="Y273" s="2"/>
+      <c r="Z273" s="2"/>
     </row>
     <row r="274" spans="1:26" ht="15.75" customHeight="1">
       <c r="A274" s="6" t="s">
         <v>732</v>
       </c>
-      <c r="B274" s="6" t="s">
+      <c r="B274" s="6"/>
+      <c r="C274" s="6" t="s">
         <v>733</v>
       </c>
-      <c r="C274" s="7" t="s">
-        <v>852</v>
-      </c>
       <c r="D274" s="6" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E274" s="6"/>
       <c r="F274" s="2"/>
@@ -12879,157 +12877,161 @@
       <c r="Z274" s="2"/>
     </row>
     <row r="275" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A275" s="8" t="s">
+      <c r="A275" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="B275" s="12"/>
+      <c r="C275" s="13" t="s">
         <v>735</v>
       </c>
-      <c r="B275" s="8"/>
-      <c r="C275" s="53" t="s">
+      <c r="D275" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="E275" s="12"/>
+      <c r="F275" s="5"/>
+      <c r="G275" s="5"/>
+      <c r="H275" s="5"/>
+      <c r="I275" s="5"/>
+      <c r="J275" s="5"/>
+      <c r="K275" s="5"/>
+      <c r="L275" s="5"/>
+      <c r="M275" s="5"/>
+      <c r="N275" s="5"/>
+      <c r="O275" s="5"/>
+      <c r="P275" s="5"/>
+      <c r="Q275" s="5"/>
+      <c r="R275" s="5"/>
+      <c r="S275" s="5"/>
+      <c r="T275" s="5"/>
+      <c r="U275" s="5"/>
+      <c r="V275" s="5"/>
+      <c r="W275" s="5"/>
+      <c r="X275" s="5"/>
+      <c r="Y275" s="5"/>
+      <c r="Z275" s="5"/>
+    </row>
+    <row r="276" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A276" s="12" t="s">
         <v>736</v>
       </c>
-      <c r="D275" s="8" t="s">
-        <v>735</v>
-      </c>
-      <c r="E275" s="6"/>
-      <c r="F275" s="2"/>
-      <c r="G275" s="2"/>
-      <c r="H275" s="2"/>
-      <c r="I275" s="2"/>
-      <c r="J275" s="2"/>
-      <c r="K275" s="2"/>
-      <c r="L275" s="2"/>
-      <c r="M275" s="2"/>
-      <c r="N275" s="2"/>
-      <c r="O275" s="2"/>
-      <c r="P275" s="2"/>
-      <c r="Q275" s="2"/>
-      <c r="R275" s="2"/>
-      <c r="S275" s="2"/>
-      <c r="T275" s="2"/>
-      <c r="U275" s="2"/>
-      <c r="V275" s="2"/>
-      <c r="W275" s="2"/>
-      <c r="X275" s="2"/>
-      <c r="Y275" s="2"/>
-      <c r="Z275" s="2"/>
-    </row>
-    <row r="276" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A276" s="6" t="s">
+      <c r="B276" s="12" t="s">
         <v>737</v>
       </c>
-      <c r="B276" s="6"/>
-      <c r="C276" s="6" t="s">
+      <c r="C276" s="13" t="s">
         <v>738</v>
       </c>
-      <c r="D276" s="6" t="s">
-        <v>737</v>
-      </c>
-      <c r="E276" s="6"/>
-      <c r="F276" s="2"/>
-      <c r="G276" s="2"/>
-      <c r="H276" s="2"/>
-      <c r="I276" s="2"/>
-      <c r="J276" s="2"/>
-      <c r="K276" s="2"/>
-      <c r="L276" s="2"/>
-      <c r="M276" s="2"/>
-      <c r="N276" s="2"/>
-      <c r="O276" s="2"/>
-      <c r="P276" s="2"/>
-      <c r="Q276" s="2"/>
-      <c r="R276" s="2"/>
-      <c r="S276" s="2"/>
-      <c r="T276" s="2"/>
-      <c r="U276" s="2"/>
-      <c r="V276" s="2"/>
-      <c r="W276" s="2"/>
-      <c r="X276" s="2"/>
-      <c r="Y276" s="2"/>
-      <c r="Z276" s="2"/>
+      <c r="D276" s="12" t="s">
+        <v>736</v>
+      </c>
+      <c r="E276" s="12"/>
+      <c r="F276" s="5"/>
+      <c r="G276" s="5"/>
+      <c r="H276" s="5"/>
+      <c r="I276" s="5"/>
+      <c r="J276" s="5"/>
+      <c r="K276" s="5"/>
+      <c r="L276" s="5"/>
+      <c r="M276" s="5"/>
+      <c r="N276" s="5"/>
+      <c r="O276" s="5"/>
+      <c r="P276" s="5"/>
+      <c r="Q276" s="5"/>
+      <c r="R276" s="5"/>
+      <c r="S276" s="5"/>
+      <c r="T276" s="5"/>
+      <c r="U276" s="5"/>
+      <c r="V276" s="5"/>
+      <c r="W276" s="5"/>
+      <c r="X276" s="5"/>
+      <c r="Y276" s="5"/>
+      <c r="Z276" s="5"/>
     </row>
     <row r="277" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A277" s="12" t="s">
+      <c r="A277" s="8" t="s">
         <v>739</v>
       </c>
-      <c r="B277" s="12"/>
-      <c r="C277" s="13" t="s">
+      <c r="B277" s="8" t="s">
         <v>740</v>
       </c>
-      <c r="D277" s="12" t="s">
+      <c r="C277" s="53" t="s">
+        <v>741</v>
+      </c>
+      <c r="D277" s="8" t="s">
         <v>739</v>
       </c>
-      <c r="E277" s="12"/>
-      <c r="F277" s="5"/>
-      <c r="G277" s="5"/>
-      <c r="H277" s="5"/>
-      <c r="I277" s="5"/>
-      <c r="J277" s="5"/>
-      <c r="K277" s="5"/>
-      <c r="L277" s="5"/>
-      <c r="M277" s="5"/>
-      <c r="N277" s="5"/>
-      <c r="O277" s="5"/>
-      <c r="P277" s="5"/>
-      <c r="Q277" s="5"/>
-      <c r="R277" s="5"/>
-      <c r="S277" s="5"/>
-      <c r="T277" s="5"/>
-      <c r="U277" s="5"/>
-      <c r="V277" s="5"/>
-      <c r="W277" s="5"/>
-      <c r="X277" s="5"/>
-      <c r="Y277" s="5"/>
-      <c r="Z277" s="5"/>
+      <c r="E277" s="8"/>
+      <c r="F277" s="2"/>
+      <c r="G277" s="2"/>
+      <c r="H277" s="2"/>
+      <c r="I277" s="2"/>
+      <c r="J277" s="2"/>
+      <c r="K277" s="2"/>
+      <c r="L277" s="2"/>
+      <c r="M277" s="2"/>
+      <c r="N277" s="2"/>
+      <c r="O277" s="2"/>
+      <c r="P277" s="2"/>
+      <c r="Q277" s="2"/>
+      <c r="R277" s="2"/>
+      <c r="S277" s="2"/>
+      <c r="T277" s="2"/>
+      <c r="U277" s="2"/>
+      <c r="V277" s="2"/>
+      <c r="W277" s="2"/>
+      <c r="X277" s="2"/>
+      <c r="Y277" s="2"/>
+      <c r="Z277" s="2"/>
     </row>
     <row r="278" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A278" s="12" t="s">
-        <v>741</v>
-      </c>
-      <c r="B278" s="12" t="s">
+      <c r="A278" s="6" t="s">
         <v>742</v>
       </c>
-      <c r="C278" s="13" t="s">
+      <c r="B278" s="6" t="s">
         <v>743</v>
       </c>
-      <c r="D278" s="12" t="s">
-        <v>741</v>
-      </c>
-      <c r="E278" s="12"/>
-      <c r="F278" s="5"/>
-      <c r="G278" s="5"/>
-      <c r="H278" s="5"/>
-      <c r="I278" s="5"/>
-      <c r="J278" s="5"/>
-      <c r="K278" s="5"/>
-      <c r="L278" s="5"/>
-      <c r="M278" s="5"/>
-      <c r="N278" s="5"/>
-      <c r="O278" s="5"/>
-      <c r="P278" s="5"/>
-      <c r="Q278" s="5"/>
-      <c r="R278" s="5"/>
-      <c r="S278" s="5"/>
-      <c r="T278" s="5"/>
-      <c r="U278" s="5"/>
-      <c r="V278" s="5"/>
-      <c r="W278" s="5"/>
-      <c r="X278" s="5"/>
-      <c r="Y278" s="5"/>
-      <c r="Z278" s="5"/>
+      <c r="C278" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="D278" s="6" t="s">
+        <v>742</v>
+      </c>
+      <c r="E278" s="6"/>
+      <c r="F278" s="2"/>
+      <c r="G278" s="2"/>
+      <c r="H278" s="2"/>
+      <c r="I278" s="2"/>
+      <c r="J278" s="2"/>
+      <c r="K278" s="2"/>
+      <c r="L278" s="2"/>
+      <c r="M278" s="2"/>
+      <c r="N278" s="2"/>
+      <c r="O278" s="2"/>
+      <c r="P278" s="2"/>
+      <c r="Q278" s="2"/>
+      <c r="R278" s="2"/>
+      <c r="S278" s="2"/>
+      <c r="T278" s="2"/>
+      <c r="U278" s="2"/>
+      <c r="V278" s="2"/>
+      <c r="W278" s="2"/>
+      <c r="X278" s="2"/>
+      <c r="Y278" s="2"/>
+      <c r="Z278" s="2"/>
     </row>
     <row r="279" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A279" s="8" t="s">
-        <v>744</v>
-      </c>
-      <c r="B279" s="8" t="s">
+      <c r="A279" s="6" t="s">
         <v>745</v>
       </c>
-      <c r="C279" s="53" t="s">
+      <c r="B279" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="C279" s="6" t="s">
         <v>746</v>
       </c>
-      <c r="D279" s="8" t="s">
-        <v>744</v>
-      </c>
-      <c r="E279" s="8"/>
+      <c r="D279" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="E279" s="6"/>
       <c r="F279" s="2"/>
       <c r="G279" s="2"/>
       <c r="H279" s="2"/>
@@ -13053,17 +13055,15 @@
       <c r="Z279" s="2"/>
     </row>
     <row r="280" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A280" s="6" t="s">
+      <c r="A280" s="8" t="s">
         <v>747</v>
       </c>
-      <c r="B280" s="6" t="s">
+      <c r="B280" s="8"/>
+      <c r="C280" s="9" t="s">
         <v>748</v>
       </c>
-      <c r="C280" s="6" t="s">
+      <c r="D280" s="8" t="s">
         <v>749</v>
-      </c>
-      <c r="D280" s="6" t="s">
-        <v>747</v>
       </c>
       <c r="E280" s="6"/>
       <c r="F280" s="2"/>
@@ -13089,16 +13089,16 @@
       <c r="Z280" s="2"/>
     </row>
     <row r="281" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A281" s="6" t="s">
+      <c r="A281" s="8" t="s">
         <v>750</v>
       </c>
-      <c r="B281" s="6" t="s">
-        <v>750</v>
-      </c>
-      <c r="C281" s="6" t="s">
+      <c r="B281" s="8" t="s">
         <v>751</v>
       </c>
-      <c r="D281" s="6" t="s">
+      <c r="C281" s="33" t="s">
+        <v>752</v>
+      </c>
+      <c r="D281" s="8" t="s">
         <v>750</v>
       </c>
       <c r="E281" s="6"/>
@@ -13125,15 +13125,17 @@
       <c r="Z281" s="2"/>
     </row>
     <row r="282" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A282" s="8" t="s">
-        <v>752</v>
-      </c>
-      <c r="B282" s="8"/>
-      <c r="C282" s="9" t="s">
+      <c r="A282" s="6" t="s">
         <v>753</v>
       </c>
-      <c r="D282" s="8" t="s">
+      <c r="B282" s="6" t="s">
         <v>754</v>
+      </c>
+      <c r="C282" s="6" t="s">
+        <v>755</v>
+      </c>
+      <c r="D282" s="6" t="s">
+        <v>753</v>
       </c>
       <c r="E282" s="6"/>
       <c r="F282" s="2"/>
@@ -13159,17 +13161,17 @@
       <c r="Z282" s="2"/>
     </row>
     <row r="283" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A283" s="8" t="s">
-        <v>755</v>
-      </c>
-      <c r="B283" s="8" t="s">
+      <c r="A283" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="C283" s="33" t="s">
+      <c r="B283" s="6" t="s">
         <v>757</v>
       </c>
-      <c r="D283" s="8" t="s">
-        <v>755</v>
+      <c r="C283" s="6" t="s">
+        <v>758</v>
+      </c>
+      <c r="D283" s="6" t="s">
+        <v>756</v>
       </c>
       <c r="E283" s="6"/>
       <c r="F283" s="2"/>
@@ -13195,17 +13197,17 @@
       <c r="Z283" s="2"/>
     </row>
     <row r="284" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A284" s="6" t="s">
-        <v>758</v>
-      </c>
-      <c r="B284" s="6" t="s">
+      <c r="A284" s="8" t="s">
         <v>759</v>
       </c>
-      <c r="C284" s="6" t="s">
+      <c r="B284" s="8" t="s">
         <v>760</v>
       </c>
-      <c r="D284" s="6" t="s">
-        <v>758</v>
+      <c r="C284" s="9" t="s">
+        <v>761</v>
+      </c>
+      <c r="D284" s="8" t="s">
+        <v>759</v>
       </c>
       <c r="E284" s="6"/>
       <c r="F284" s="2"/>
@@ -13231,19 +13233,17 @@
       <c r="Z284" s="2"/>
     </row>
     <row r="285" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A285" s="6" t="s">
-        <v>761</v>
-      </c>
-      <c r="B285" s="6" t="s">
+      <c r="A285" s="10" t="s">
         <v>762</v>
       </c>
-      <c r="C285" s="6" t="s">
+      <c r="B285" s="10"/>
+      <c r="C285" s="34" t="s">
         <v>763</v>
       </c>
-      <c r="D285" s="6" t="s">
-        <v>761</v>
-      </c>
-      <c r="E285" s="6"/>
+      <c r="D285" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="E285" s="10"/>
       <c r="F285" s="2"/>
       <c r="G285" s="2"/>
       <c r="H285" s="2"/>
@@ -13267,17 +13267,17 @@
       <c r="Z285" s="2"/>
     </row>
     <row r="286" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A286" s="8" t="s">
-        <v>764</v>
-      </c>
-      <c r="B286" s="8" t="s">
+      <c r="A286" s="6" t="s">
         <v>765</v>
       </c>
-      <c r="C286" s="9" t="s">
+      <c r="B286" s="6" t="s">
         <v>766</v>
       </c>
-      <c r="D286" s="8" t="s">
-        <v>764</v>
+      <c r="C286" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="D286" s="6" t="s">
+        <v>765</v>
       </c>
       <c r="E286" s="6"/>
       <c r="F286" s="2"/>
@@ -13303,17 +13303,19 @@
       <c r="Z286" s="2"/>
     </row>
     <row r="287" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A287" s="10" t="s">
-        <v>767</v>
-      </c>
-      <c r="B287" s="10"/>
-      <c r="C287" s="34" t="s">
+      <c r="A287" s="8" t="s">
         <v>768</v>
       </c>
-      <c r="D287" s="10" t="s">
+      <c r="B287" s="8" t="s">
         <v>769</v>
       </c>
-      <c r="E287" s="10"/>
+      <c r="C287" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="D287" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="E287" s="6"/>
       <c r="F287" s="2"/>
       <c r="G287" s="2"/>
       <c r="H287" s="2"/>
@@ -13338,16 +13340,16 @@
     </row>
     <row r="288" spans="1:26" ht="15.75" customHeight="1">
       <c r="A288" s="6" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B288" s="6" t="s">
-        <v>771</v>
-      </c>
-      <c r="C288" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="C288" s="7" t="s">
+        <v>774</v>
+      </c>
+      <c r="D288" s="6" t="s">
         <v>772</v>
-      </c>
-      <c r="D288" s="6" t="s">
-        <v>770</v>
       </c>
       <c r="E288" s="6"/>
       <c r="F288" s="2"/>
@@ -13373,76 +13375,74 @@
       <c r="Z288" s="2"/>
     </row>
     <row r="289" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A289" s="8" t="s">
-        <v>773</v>
-      </c>
-      <c r="B289" s="8" t="s">
-        <v>774</v>
-      </c>
-      <c r="C289" s="9" t="s">
+      <c r="A289" s="12" t="s">
         <v>775</v>
       </c>
-      <c r="D289" s="8" t="s">
+      <c r="B289" s="12"/>
+      <c r="C289" s="14" t="s">
         <v>776</v>
       </c>
-      <c r="E289" s="6"/>
-      <c r="F289" s="2"/>
-      <c r="G289" s="2"/>
-      <c r="H289" s="2"/>
-      <c r="I289" s="2"/>
-      <c r="J289" s="2"/>
-      <c r="K289" s="2"/>
-      <c r="L289" s="2"/>
-      <c r="M289" s="2"/>
-      <c r="N289" s="2"/>
-      <c r="O289" s="2"/>
-      <c r="P289" s="2"/>
-      <c r="Q289" s="2"/>
-      <c r="R289" s="2"/>
-      <c r="S289" s="2"/>
-      <c r="T289" s="2"/>
-      <c r="U289" s="2"/>
-      <c r="V289" s="2"/>
-      <c r="W289" s="2"/>
-      <c r="X289" s="2"/>
-      <c r="Y289" s="2"/>
-      <c r="Z289" s="2"/>
+      <c r="D289" s="12" t="s">
+        <v>775</v>
+      </c>
+      <c r="E289" s="12"/>
+      <c r="F289" s="5"/>
+      <c r="G289" s="5"/>
+      <c r="H289" s="5"/>
+      <c r="I289" s="5"/>
+      <c r="J289" s="5"/>
+      <c r="K289" s="5"/>
+      <c r="L289" s="5"/>
+      <c r="M289" s="5"/>
+      <c r="N289" s="5"/>
+      <c r="O289" s="5"/>
+      <c r="P289" s="5"/>
+      <c r="Q289" s="5"/>
+      <c r="R289" s="5"/>
+      <c r="S289" s="5"/>
+      <c r="T289" s="5"/>
+      <c r="U289" s="5"/>
+      <c r="V289" s="5"/>
+      <c r="W289" s="5"/>
+      <c r="X289" s="5"/>
+      <c r="Y289" s="5"/>
+      <c r="Z289" s="5"/>
     </row>
     <row r="290" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A290" s="6" t="s">
+      <c r="A290" s="12" t="s">
         <v>777</v>
       </c>
-      <c r="B290" s="6" t="s">
+      <c r="B290" s="12" t="s">
         <v>778</v>
       </c>
-      <c r="C290" s="7" t="s">
+      <c r="C290" s="13" t="s">
         <v>779</v>
       </c>
-      <c r="D290" s="6" t="s">
+      <c r="D290" s="12" t="s">
         <v>777</v>
       </c>
-      <c r="E290" s="6"/>
-      <c r="F290" s="2"/>
-      <c r="G290" s="2"/>
-      <c r="H290" s="2"/>
-      <c r="I290" s="2"/>
-      <c r="J290" s="2"/>
-      <c r="K290" s="2"/>
-      <c r="L290" s="2"/>
-      <c r="M290" s="2"/>
-      <c r="N290" s="2"/>
-      <c r="O290" s="2"/>
-      <c r="P290" s="2"/>
-      <c r="Q290" s="2"/>
-      <c r="R290" s="2"/>
-      <c r="S290" s="2"/>
-      <c r="T290" s="2"/>
-      <c r="U290" s="2"/>
-      <c r="V290" s="2"/>
-      <c r="W290" s="2"/>
-      <c r="X290" s="2"/>
-      <c r="Y290" s="2"/>
-      <c r="Z290" s="2"/>
+      <c r="E290" s="12"/>
+      <c r="F290" s="5"/>
+      <c r="G290" s="5"/>
+      <c r="H290" s="5"/>
+      <c r="I290" s="5"/>
+      <c r="J290" s="5"/>
+      <c r="K290" s="5"/>
+      <c r="L290" s="5"/>
+      <c r="M290" s="5"/>
+      <c r="N290" s="5"/>
+      <c r="O290" s="5"/>
+      <c r="P290" s="5"/>
+      <c r="Q290" s="5"/>
+      <c r="R290" s="5"/>
+      <c r="S290" s="5"/>
+      <c r="T290" s="5"/>
+      <c r="U290" s="5"/>
+      <c r="V290" s="5"/>
+      <c r="W290" s="5"/>
+      <c r="X290" s="5"/>
+      <c r="Y290" s="5"/>
+      <c r="Z290" s="5"/>
     </row>
     <row r="291" spans="1:26" ht="15.75" customHeight="1">
       <c r="A291" s="12" t="s">
@@ -13453,7 +13453,7 @@
         <v>781</v>
       </c>
       <c r="D291" s="12" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="E291" s="12"/>
       <c r="F291" s="5"/>
@@ -13479,85 +13479,87 @@
       <c r="Z291" s="5"/>
     </row>
     <row r="292" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A292" s="12" t="s">
-        <v>782</v>
-      </c>
-      <c r="B292" s="12" t="s">
+      <c r="A292" s="10" t="s">
         <v>783</v>
       </c>
-      <c r="C292" s="13" t="s">
+      <c r="B292" s="10"/>
+      <c r="C292" s="11" t="s">
         <v>784</v>
       </c>
-      <c r="D292" s="12" t="s">
-        <v>782</v>
-      </c>
-      <c r="E292" s="12"/>
-      <c r="F292" s="5"/>
-      <c r="G292" s="5"/>
-      <c r="H292" s="5"/>
-      <c r="I292" s="5"/>
-      <c r="J292" s="5"/>
-      <c r="K292" s="5"/>
-      <c r="L292" s="5"/>
-      <c r="M292" s="5"/>
-      <c r="N292" s="5"/>
-      <c r="O292" s="5"/>
-      <c r="P292" s="5"/>
-      <c r="Q292" s="5"/>
-      <c r="R292" s="5"/>
-      <c r="S292" s="5"/>
-      <c r="T292" s="5"/>
-      <c r="U292" s="5"/>
-      <c r="V292" s="5"/>
-      <c r="W292" s="5"/>
-      <c r="X292" s="5"/>
-      <c r="Y292" s="5"/>
-      <c r="Z292" s="5"/>
+      <c r="D292" s="10"/>
+      <c r="E292" s="10"/>
+      <c r="F292" s="2"/>
+      <c r="G292" s="2"/>
+      <c r="H292" s="2"/>
+      <c r="I292" s="2"/>
+      <c r="J292" s="2"/>
+      <c r="K292" s="2"/>
+      <c r="L292" s="2"/>
+      <c r="M292" s="2"/>
+      <c r="N292" s="2"/>
+      <c r="O292" s="2"/>
+      <c r="P292" s="2"/>
+      <c r="Q292" s="2"/>
+      <c r="R292" s="2"/>
+      <c r="S292" s="2"/>
+      <c r="T292" s="2"/>
+      <c r="U292" s="2"/>
+      <c r="V292" s="2"/>
+      <c r="W292" s="2"/>
+      <c r="X292" s="2"/>
+      <c r="Y292" s="2"/>
+      <c r="Z292" s="2"/>
     </row>
     <row r="293" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A293" s="12" t="s">
+      <c r="A293" s="10" t="s">
         <v>785</v>
       </c>
-      <c r="B293" s="12"/>
-      <c r="C293" s="14" t="s">
+      <c r="B293" s="10" t="s">
         <v>786</v>
       </c>
-      <c r="D293" s="12" t="s">
+      <c r="C293" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D293" s="10" t="s">
         <v>787</v>
       </c>
-      <c r="E293" s="12"/>
-      <c r="F293" s="5"/>
-      <c r="G293" s="5"/>
-      <c r="H293" s="5"/>
-      <c r="I293" s="5"/>
-      <c r="J293" s="5"/>
-      <c r="K293" s="5"/>
-      <c r="L293" s="5"/>
-      <c r="M293" s="5"/>
-      <c r="N293" s="5"/>
-      <c r="O293" s="5"/>
-      <c r="P293" s="5"/>
-      <c r="Q293" s="5"/>
-      <c r="R293" s="5"/>
-      <c r="S293" s="5"/>
-      <c r="T293" s="5"/>
-      <c r="U293" s="5"/>
-      <c r="V293" s="5"/>
-      <c r="W293" s="5"/>
-      <c r="X293" s="5"/>
-      <c r="Y293" s="5"/>
-      <c r="Z293" s="5"/>
+      <c r="E293" s="10"/>
+      <c r="F293" s="2"/>
+      <c r="G293" s="2"/>
+      <c r="H293" s="2"/>
+      <c r="I293" s="2"/>
+      <c r="J293" s="2"/>
+      <c r="K293" s="2"/>
+      <c r="L293" s="2"/>
+      <c r="M293" s="2"/>
+      <c r="N293" s="2"/>
+      <c r="O293" s="2"/>
+      <c r="P293" s="2"/>
+      <c r="Q293" s="2"/>
+      <c r="R293" s="2"/>
+      <c r="S293" s="2"/>
+      <c r="T293" s="2"/>
+      <c r="U293" s="2"/>
+      <c r="V293" s="2"/>
+      <c r="W293" s="2"/>
+      <c r="X293" s="2"/>
+      <c r="Y293" s="2"/>
+      <c r="Z293" s="2"/>
     </row>
     <row r="294" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A294" s="10" t="s">
+      <c r="A294" s="6" t="s">
         <v>788</v>
       </c>
-      <c r="B294" s="10"/>
-      <c r="C294" s="11" t="s">
+      <c r="B294" s="6" t="s">
         <v>789</v>
       </c>
-      <c r="D294" s="10"/>
-      <c r="E294" s="10"/>
+      <c r="C294" s="15" t="s">
+        <v>790</v>
+      </c>
+      <c r="D294" s="6" t="s">
+        <v>791</v>
+      </c>
+      <c r="E294" s="6"/>
       <c r="F294" s="2"/>
       <c r="G294" s="2"/>
       <c r="H294" s="2"/>
@@ -13581,19 +13583,17 @@
       <c r="Z294" s="2"/>
     </row>
     <row r="295" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A295" s="10" t="s">
-        <v>790</v>
-      </c>
-      <c r="B295" s="10" t="s">
-        <v>791</v>
-      </c>
-      <c r="C295" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D295" s="10" t="s">
+      <c r="A295" s="8" t="s">
         <v>792</v>
       </c>
-      <c r="E295" s="10"/>
+      <c r="B295" s="8"/>
+      <c r="C295" s="9" t="s">
+        <v>793</v>
+      </c>
+      <c r="D295" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="E295" s="8"/>
       <c r="F295" s="2"/>
       <c r="G295" s="2"/>
       <c r="H295" s="2"/>
@@ -13617,19 +13617,17 @@
       <c r="Z295" s="2"/>
     </row>
     <row r="296" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A296" s="6" t="s">
-        <v>793</v>
-      </c>
-      <c r="B296" s="6" t="s">
+      <c r="A296" s="8" t="s">
         <v>794</v>
       </c>
-      <c r="C296" s="15" t="s">
+      <c r="B296" s="8"/>
+      <c r="C296" s="9" t="s">
         <v>795</v>
       </c>
-      <c r="D296" s="6" t="s">
+      <c r="D296" s="8" t="s">
         <v>796</v>
       </c>
-      <c r="E296" s="6"/>
+      <c r="E296" s="8"/>
       <c r="F296" s="2"/>
       <c r="G296" s="2"/>
       <c r="H296" s="2"/>
@@ -13724,12 +13722,14 @@
       <c r="A299" s="8" t="s">
         <v>802</v>
       </c>
-      <c r="B299" s="8"/>
+      <c r="B299" s="8" t="s">
+        <v>803</v>
+      </c>
       <c r="C299" s="9" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="D299" s="8" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="E299" s="8"/>
       <c r="F299" s="2"/>
@@ -13756,14 +13756,14 @@
     </row>
     <row r="300" spans="1:26" ht="15.75" customHeight="1">
       <c r="A300" s="8" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="B300" s="8"/>
       <c r="C300" s="9" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="D300" s="8" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="E300" s="8"/>
       <c r="F300" s="2"/>
@@ -13789,17 +13789,15 @@
       <c r="Z300" s="2"/>
     </row>
     <row r="301" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A301" s="8" t="s">
-        <v>807</v>
-      </c>
-      <c r="B301" s="8" t="s">
-        <v>808</v>
-      </c>
-      <c r="C301" s="9" t="s">
+      <c r="A301" s="10" t="s">
         <v>809</v>
       </c>
-      <c r="D301" s="8" t="s">
+      <c r="B301" s="10"/>
+      <c r="C301" s="11" t="s">
         <v>810</v>
+      </c>
+      <c r="D301" s="10" t="s">
+        <v>809</v>
       </c>
       <c r="E301" s="8"/>
       <c r="F301" s="2"/>
@@ -13833,7 +13831,7 @@
         <v>812</v>
       </c>
       <c r="D302" s="8" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E302" s="8"/>
       <c r="F302" s="2"/>
@@ -13859,15 +13857,17 @@
       <c r="Z302" s="2"/>
     </row>
     <row r="303" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A303" s="10" t="s">
+      <c r="A303" s="8" t="s">
+        <v>813</v>
+      </c>
+      <c r="B303" s="8" t="s">
         <v>814</v>
       </c>
-      <c r="B303" s="10"/>
-      <c r="C303" s="11" t="s">
+      <c r="C303" s="9" t="s">
         <v>815</v>
       </c>
-      <c r="D303" s="10" t="s">
-        <v>814</v>
+      <c r="D303" s="8" t="s">
+        <v>813</v>
       </c>
       <c r="E303" s="8"/>
       <c r="F303" s="2"/>
@@ -13893,17 +13893,17 @@
       <c r="Z303" s="2"/>
     </row>
     <row r="304" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A304" s="8" t="s">
+      <c r="A304" s="6" t="s">
         <v>816</v>
       </c>
-      <c r="B304" s="8"/>
-      <c r="C304" s="9" t="s">
+      <c r="B304" s="6"/>
+      <c r="C304" s="15" t="s">
         <v>817</v>
       </c>
-      <c r="D304" s="8" t="s">
+      <c r="D304" s="6" t="s">
         <v>816</v>
       </c>
-      <c r="E304" s="8"/>
+      <c r="E304" s="6"/>
       <c r="F304" s="2"/>
       <c r="G304" s="2"/>
       <c r="H304" s="2"/>
@@ -13927,121 +13927,123 @@
       <c r="Z304" s="2"/>
     </row>
     <row r="305" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A305" s="8" t="s">
+      <c r="A305" s="12" t="s">
         <v>818</v>
       </c>
-      <c r="B305" s="8" t="s">
+      <c r="B305" s="12"/>
+      <c r="C305" s="13" t="s">
         <v>819</v>
       </c>
-      <c r="C305" s="9" t="s">
+      <c r="D305" s="12" t="s">
         <v>820</v>
       </c>
-      <c r="D305" s="8" t="s">
-        <v>818</v>
-      </c>
-      <c r="E305" s="8"/>
-      <c r="F305" s="2"/>
-      <c r="G305" s="2"/>
-      <c r="H305" s="2"/>
-      <c r="I305" s="2"/>
-      <c r="J305" s="2"/>
-      <c r="K305" s="2"/>
-      <c r="L305" s="2"/>
-      <c r="M305" s="2"/>
-      <c r="N305" s="2"/>
-      <c r="O305" s="2"/>
-      <c r="P305" s="2"/>
-      <c r="Q305" s="2"/>
-      <c r="R305" s="2"/>
-      <c r="S305" s="2"/>
-      <c r="T305" s="2"/>
-      <c r="U305" s="2"/>
-      <c r="V305" s="2"/>
-      <c r="W305" s="2"/>
-      <c r="X305" s="2"/>
-      <c r="Y305" s="2"/>
-      <c r="Z305" s="2"/>
+      <c r="E305" s="12"/>
+      <c r="F305" s="5"/>
+      <c r="G305" s="5"/>
+      <c r="H305" s="5"/>
+      <c r="I305" s="5"/>
+      <c r="J305" s="5"/>
+      <c r="K305" s="5"/>
+      <c r="L305" s="5"/>
+      <c r="M305" s="5"/>
+      <c r="N305" s="5"/>
+      <c r="O305" s="5"/>
+      <c r="P305" s="5"/>
+      <c r="Q305" s="5"/>
+      <c r="R305" s="5"/>
+      <c r="S305" s="5"/>
+      <c r="T305" s="5"/>
+      <c r="U305" s="5"/>
+      <c r="V305" s="5"/>
+      <c r="W305" s="5"/>
+      <c r="X305" s="5"/>
+      <c r="Y305" s="5"/>
+      <c r="Z305" s="5"/>
     </row>
     <row r="306" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A306" s="6" t="s">
+      <c r="A306" s="12" t="s">
         <v>821</v>
       </c>
-      <c r="B306" s="6"/>
-      <c r="C306" s="15" t="s">
+      <c r="B306" s="12" t="s">
         <v>822</v>
       </c>
-      <c r="D306" s="6" t="s">
+      <c r="C306" s="14" t="s">
+        <v>823</v>
+      </c>
+      <c r="D306" s="12" t="s">
         <v>821</v>
       </c>
-      <c r="E306" s="6"/>
-      <c r="F306" s="2"/>
-      <c r="G306" s="2"/>
-      <c r="H306" s="2"/>
-      <c r="I306" s="2"/>
-      <c r="J306" s="2"/>
-      <c r="K306" s="2"/>
-      <c r="L306" s="2"/>
-      <c r="M306" s="2"/>
-      <c r="N306" s="2"/>
-      <c r="O306" s="2"/>
-      <c r="P306" s="2"/>
-      <c r="Q306" s="2"/>
-      <c r="R306" s="2"/>
-      <c r="S306" s="2"/>
-      <c r="T306" s="2"/>
-      <c r="U306" s="2"/>
-      <c r="V306" s="2"/>
-      <c r="W306" s="2"/>
-      <c r="X306" s="2"/>
-      <c r="Y306" s="2"/>
-      <c r="Z306" s="2"/>
+      <c r="E306" s="12"/>
+      <c r="F306" s="5"/>
+      <c r="G306" s="5"/>
+      <c r="H306" s="5"/>
+      <c r="I306" s="5"/>
+      <c r="J306" s="5"/>
+      <c r="K306" s="5"/>
+      <c r="L306" s="5"/>
+      <c r="M306" s="5"/>
+      <c r="N306" s="5"/>
+      <c r="O306" s="5"/>
+      <c r="P306" s="5"/>
+      <c r="Q306" s="5"/>
+      <c r="R306" s="5"/>
+      <c r="S306" s="5"/>
+      <c r="T306" s="5"/>
+      <c r="U306" s="5"/>
+      <c r="V306" s="5"/>
+      <c r="W306" s="5"/>
+      <c r="X306" s="5"/>
+      <c r="Y306" s="5"/>
+      <c r="Z306" s="5"/>
     </row>
     <row r="307" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A307" s="12" t="s">
-        <v>823</v>
-      </c>
-      <c r="B307" s="12"/>
-      <c r="C307" s="13" t="s">
+      <c r="A307" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="D307" s="12" t="s">
+      <c r="B307" s="6" t="s">
         <v>825</v>
       </c>
-      <c r="E307" s="12"/>
-      <c r="F307" s="5"/>
-      <c r="G307" s="5"/>
-      <c r="H307" s="5"/>
-      <c r="I307" s="5"/>
-      <c r="J307" s="5"/>
-      <c r="K307" s="5"/>
-      <c r="L307" s="5"/>
-      <c r="M307" s="5"/>
-      <c r="N307" s="5"/>
-      <c r="O307" s="5"/>
-      <c r="P307" s="5"/>
-      <c r="Q307" s="5"/>
-      <c r="R307" s="5"/>
-      <c r="S307" s="5"/>
-      <c r="T307" s="5"/>
-      <c r="U307" s="5"/>
-      <c r="V307" s="5"/>
-      <c r="W307" s="5"/>
-      <c r="X307" s="5"/>
-      <c r="Y307" s="5"/>
-      <c r="Z307" s="5"/>
+      <c r="C307" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="D307" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="E307" s="6"/>
+      <c r="F307" s="2"/>
+      <c r="G307" s="2"/>
+      <c r="H307" s="2"/>
+      <c r="I307" s="2"/>
+      <c r="J307" s="2"/>
+      <c r="K307" s="2"/>
+      <c r="L307" s="2"/>
+      <c r="M307" s="2"/>
+      <c r="N307" s="2"/>
+      <c r="O307" s="2"/>
+      <c r="P307" s="2"/>
+      <c r="Q307" s="2"/>
+      <c r="R307" s="2"/>
+      <c r="S307" s="2"/>
+      <c r="T307" s="2"/>
+      <c r="U307" s="2"/>
+      <c r="V307" s="2"/>
+      <c r="W307" s="2"/>
+      <c r="X307" s="2"/>
+      <c r="Y307" s="2"/>
+      <c r="Z307" s="2"/>
     </row>
     <row r="308" spans="1:26" ht="15.75" customHeight="1">
       <c r="A308" s="12" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B308" s="12" t="s">
+        <v>828</v>
+      </c>
+      <c r="C308" s="13" t="s">
+        <v>829</v>
+      </c>
+      <c r="D308" s="12" t="s">
         <v>827</v>
-      </c>
-      <c r="C308" s="14" t="s">
-        <v>828</v>
-      </c>
-      <c r="D308" s="12" t="s">
-        <v>826</v>
       </c>
       <c r="E308" s="12"/>
       <c r="F308" s="5"/>
@@ -14068,16 +14070,14 @@
     </row>
     <row r="309" spans="1:26" ht="15.75" customHeight="1">
       <c r="A309" s="6" t="s">
-        <v>829</v>
-      </c>
-      <c r="B309" s="6" t="s">
         <v>830</v>
       </c>
+      <c r="B309" s="6"/>
       <c r="C309" s="7" t="s">
         <v>831</v>
       </c>
       <c r="D309" s="6" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E309" s="6"/>
       <c r="F309" s="2"/>
@@ -14103,53 +14103,53 @@
       <c r="Z309" s="2"/>
     </row>
     <row r="310" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A310" s="12" t="s">
+      <c r="A310" s="8" t="s">
         <v>832</v>
       </c>
-      <c r="B310" s="12" t="s">
+      <c r="B310" s="8"/>
+      <c r="C310" s="9" t="s">
         <v>833</v>
       </c>
-      <c r="C310" s="13" t="s">
-        <v>834</v>
-      </c>
-      <c r="D310" s="12" t="s">
+      <c r="D310" s="54" t="s">
         <v>832</v>
       </c>
-      <c r="E310" s="12"/>
-      <c r="F310" s="5"/>
-      <c r="G310" s="5"/>
-      <c r="H310" s="5"/>
-      <c r="I310" s="5"/>
-      <c r="J310" s="5"/>
-      <c r="K310" s="5"/>
-      <c r="L310" s="5"/>
-      <c r="M310" s="5"/>
-      <c r="N310" s="5"/>
-      <c r="O310" s="5"/>
-      <c r="P310" s="5"/>
-      <c r="Q310" s="5"/>
-      <c r="R310" s="5"/>
-      <c r="S310" s="5"/>
-      <c r="T310" s="5"/>
-      <c r="U310" s="5"/>
-      <c r="V310" s="5"/>
-      <c r="W310" s="5"/>
-      <c r="X310" s="5"/>
-      <c r="Y310" s="5"/>
-      <c r="Z310" s="5"/>
+      <c r="E310" s="54"/>
+      <c r="F310" s="2"/>
+      <c r="G310" s="2"/>
+      <c r="H310" s="2"/>
+      <c r="I310" s="2"/>
+      <c r="J310" s="2"/>
+      <c r="K310" s="2"/>
+      <c r="L310" s="2"/>
+      <c r="M310" s="2"/>
+      <c r="N310" s="2"/>
+      <c r="O310" s="2"/>
+      <c r="P310" s="2"/>
+      <c r="Q310" s="2"/>
+      <c r="R310" s="2"/>
+      <c r="S310" s="2"/>
+      <c r="T310" s="2"/>
+      <c r="U310" s="2"/>
+      <c r="V310" s="2"/>
+      <c r="W310" s="2"/>
+      <c r="X310" s="2"/>
+      <c r="Y310" s="2"/>
+      <c r="Z310" s="2"/>
     </row>
     <row r="311" spans="1:26" ht="15.75" customHeight="1">
       <c r="A311" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="B311" s="6" t="s">
         <v>835</v>
       </c>
-      <c r="B311" s="6"/>
-      <c r="C311" s="7" t="s">
+      <c r="C311" s="15" t="s">
         <v>836</v>
       </c>
-      <c r="D311" s="6" t="s">
-        <v>835</v>
-      </c>
-      <c r="E311" s="6"/>
+      <c r="D311" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="E311" s="2"/>
       <c r="F311" s="2"/>
       <c r="G311" s="2"/>
       <c r="H311" s="2"/>
@@ -14180,80 +14180,22 @@
       <c r="C312" s="9" t="s">
         <v>838</v>
       </c>
-      <c r="D312" s="54" t="s">
-        <v>837</v>
-      </c>
-      <c r="E312" s="54"/>
-      <c r="F312" s="2"/>
-      <c r="G312" s="2"/>
-      <c r="H312" s="2"/>
-      <c r="I312" s="2"/>
-      <c r="J312" s="2"/>
-      <c r="K312" s="2"/>
-      <c r="L312" s="2"/>
-      <c r="M312" s="2"/>
-      <c r="N312" s="2"/>
-      <c r="O312" s="2"/>
-      <c r="P312" s="2"/>
-      <c r="Q312" s="2"/>
-      <c r="R312" s="2"/>
-      <c r="S312" s="2"/>
-      <c r="T312" s="2"/>
-      <c r="U312" s="2"/>
-      <c r="V312" s="2"/>
-      <c r="W312" s="2"/>
-      <c r="X312" s="2"/>
-      <c r="Y312" s="2"/>
-      <c r="Z312" s="2"/>
+      <c r="D312" s="55" t="s">
+        <v>839</v>
+      </c>
+      <c r="E312" s="55"/>
     </row>
     <row r="313" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A313" s="6" t="s">
-        <v>839</v>
-      </c>
-      <c r="B313" s="6" t="s">
-        <v>840</v>
-      </c>
-      <c r="C313" s="15" t="s">
-        <v>841</v>
-      </c>
-      <c r="D313" s="2" t="s">
-        <v>839</v>
-      </c>
-      <c r="E313" s="2"/>
-      <c r="F313" s="2"/>
-      <c r="G313" s="2"/>
-      <c r="H313" s="2"/>
-      <c r="I313" s="2"/>
-      <c r="J313" s="2"/>
-      <c r="K313" s="2"/>
-      <c r="L313" s="2"/>
-      <c r="M313" s="2"/>
-      <c r="N313" s="2"/>
-      <c r="O313" s="2"/>
-      <c r="P313" s="2"/>
-      <c r="Q313" s="2"/>
-      <c r="R313" s="2"/>
-      <c r="S313" s="2"/>
-      <c r="T313" s="2"/>
-      <c r="U313" s="2"/>
-      <c r="V313" s="2"/>
-      <c r="W313" s="2"/>
-      <c r="X313" s="2"/>
-      <c r="Y313" s="2"/>
-      <c r="Z313" s="2"/>
+      <c r="A313" s="6"/>
+      <c r="B313" s="6"/>
+      <c r="C313" s="6"/>
+      <c r="D313" s="2"/>
     </row>
     <row r="314" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A314" s="8" t="s">
-        <v>842</v>
-      </c>
-      <c r="B314" s="8"/>
-      <c r="C314" s="9" t="s">
-        <v>843</v>
-      </c>
-      <c r="D314" s="55" t="s">
-        <v>844</v>
-      </c>
-      <c r="E314" s="55"/>
+      <c r="A314" s="6"/>
+      <c r="B314" s="6"/>
+      <c r="C314" s="6"/>
+      <c r="D314" s="2"/>
     </row>
     <row r="315" spans="1:26" ht="15.75" customHeight="1">
       <c r="A315" s="6"/>
@@ -19702,18 +19644,6 @@
       <c r="B1222" s="6"/>
       <c r="C1222" s="6"/>
       <c r="D1222" s="2"/>
-    </row>
-    <row r="1223" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1223" s="6"/>
-      <c r="B1223" s="6"/>
-      <c r="C1223" s="6"/>
-      <c r="D1223" s="2"/>
-    </row>
-    <row r="1224" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1224" s="6"/>
-      <c r="B1224" s="6"/>
-      <c r="C1224" s="6"/>
-      <c r="D1224" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -19850,106 +19780,106 @@
     <hyperlink ref="C164" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
     <hyperlink ref="C165" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
     <hyperlink ref="C166" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="C167" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="C170" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="C173" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="C176" r:id="rId137" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="C177" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="C178" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="C180" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="C181" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="C182" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="C184" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="C186" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="C187" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="C188" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="C189" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="C190" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="C192" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="C194" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="C195" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="C196" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="C198" r:id="rId153" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="C200" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="C201" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="C202" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="C206" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="C207" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="C209" r:id="rId159" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="C210" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="C212" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="C213" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="C214" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="C216" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="C217" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="C220" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="C221" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="C223" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="C224" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="C225" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="C226" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="C228" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="C231" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="C232" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="C233" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="C235" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="C236" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="C237" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="C238" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="C241" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="C243" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="C244" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="C245" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="C246" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="C247" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="C249" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="C250" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="C252" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="C255" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="C256" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="C257" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="C258" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="C260" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="C261" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="C262" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="C264" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="C265" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="C269" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="C270" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="C271" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="C273" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="C275" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="C277" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="C279" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="C282" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="C283" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="C286" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="C287" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="C289" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="C290" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="C291" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="C293" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="C294" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="C295" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="C296" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="C297" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="C298" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="C299" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="C300" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="C301" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="C302" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="C303" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="C304" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="C305" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="C306" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="C308" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="C309" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="C311" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="C312" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="C313" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="C314" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="C130" r:id="rId232" xr:uid="{98DDE684-CC21-7C49-B22B-C4F92C88FD93}"/>
-    <hyperlink ref="C172" r:id="rId233" xr:uid="{E941C717-9955-3748-A705-A152EB86702B}"/>
+    <hyperlink ref="C170" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="C173" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="C176" r:id="rId136" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="C177" r:id="rId137" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="C178" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="C180" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="C181" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="C182" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="C184" r:id="rId142" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="C186" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="C187" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="C188" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="C189" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="C190" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="C192" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="C194" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="C195" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="C196" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="C198" r:id="rId152" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="C200" r:id="rId153" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="C201" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="C202" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="C206" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="C207" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="C209" r:id="rId158" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="C210" r:id="rId159" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="C211" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="C212" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="C213" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="C215" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="C216" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="C219" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="C220" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="C222" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="C223" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="C224" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="C225" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="C227" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="C230" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="C231" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="C232" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="C234" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="C235" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="C236" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="C237" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="C240" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="C241" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="C242" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="C243" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="C244" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="C245" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="C247" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="C248" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="C250" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="C253" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="C254" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="C255" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="C256" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="C258" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="C259" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="C260" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="C262" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="C263" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="C267" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="C268" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="C269" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="C271" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="C273" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="C275" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="C277" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="C280" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="C281" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="C284" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="C285" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="C287" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="C288" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="C289" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="C291" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="C292" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="C293" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="C294" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="C295" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="C296" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="C297" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="C298" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="C299" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="C300" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="C301" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="C302" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="C303" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="C304" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="C306" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="C307" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="C309" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="C310" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="C311" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="C312" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="C130" r:id="rId231" xr:uid="{98DDE684-CC21-7C49-B22B-C4F92C88FD93}"/>
+    <hyperlink ref="C172" r:id="rId232" xr:uid="{E941C717-9955-3748-A705-A152EB86702B}"/>
+    <hyperlink ref="C203" r:id="rId233" xr:uid="{E097DAE9-B813-AD4F-99E1-6F78BF720202}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Correction according to list
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Ortsregister_2023.xlsx
+++ b/data/xlsx/Baernreither_Ortsregister_2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B985574-6997-BA41-81D0-10C45236BCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F875124-4333-EC42-8C07-04CB5707764C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3308,8 +3308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="169" workbookViewId="0">
-      <selection activeCell="A241" sqref="A241:XFD241"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="D203" sqref="D203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -19879,7 +19879,7 @@
     <hyperlink ref="C312" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
     <hyperlink ref="C130" r:id="rId231" xr:uid="{98DDE684-CC21-7C49-B22B-C4F92C88FD93}"/>
     <hyperlink ref="C172" r:id="rId232" xr:uid="{E941C717-9955-3748-A705-A152EB86702B}"/>
-    <hyperlink ref="C203" r:id="rId233" xr:uid="{E097DAE9-B813-AD4F-99E1-6F78BF720202}"/>
+    <hyperlink ref="C203" r:id="rId233" xr:uid="{35225AD0-6E86-F842-9A7D-130AABE12B66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>